<commit_message>
memory drills update, added interesting links and blueprint checklist
</commit_message>
<xml_diff>
--- a/written-exam-memory-drills.xlsx
+++ b/written-exam-memory-drills.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13080" yWindow="1020" windowWidth="25600" windowHeight="15620" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="3680" yWindow="260" windowWidth="30260" windowHeight="19960" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="fill-in" sheetId="1" r:id="rId1"/>
     <sheet name="answers" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2130" uniqueCount="1360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2135" uniqueCount="1363">
   <si>
     <t>bgp best-path</t>
   </si>
@@ -4161,12 +4161,21 @@
   <si>
     <t>discard</t>
   </si>
+  <si>
+    <t>pim defaults</t>
+  </si>
+  <si>
+    <t>hold time</t>
+  </si>
+  <si>
+    <t>105 (1:45)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -4224,6 +4233,18 @@
       <b/>
       <sz val="11"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="7">
@@ -4295,10 +4316,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4414,12 +4439,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -8708,8 +8738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P32" workbookViewId="0">
-      <selection activeCell="U50" sqref="U50"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
+      <selection activeCell="AK12" sqref="AK12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -9024,10 +9054,10 @@
       <c r="AS3" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="AT3" s="79" t="s">
+      <c r="AT3" s="80" t="s">
         <v>82</v>
       </c>
-      <c r="AU3" s="80"/>
+      <c r="AU3" s="81"/>
     </row>
     <row r="4" spans="1:47" ht="14.25" customHeight="1">
       <c r="A4" s="5" t="s">
@@ -9104,10 +9134,10 @@
       <c r="AQ4" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="AS4" s="79" t="s">
+      <c r="AS4" s="80" t="s">
         <v>116</v>
       </c>
-      <c r="AT4" s="80"/>
+      <c r="AT4" s="81"/>
       <c r="AU4" s="14"/>
     </row>
     <row r="5" spans="1:47" ht="14.25" customHeight="1">
@@ -9156,10 +9186,10 @@
       <c r="AS5" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="AT5" s="79" t="s">
+      <c r="AT5" s="80" t="s">
         <v>128</v>
       </c>
-      <c r="AU5" s="80"/>
+      <c r="AU5" s="81"/>
     </row>
     <row r="6" spans="1:47" ht="14.25" customHeight="1">
       <c r="A6" s="5" t="s">
@@ -9610,13 +9640,15 @@
       <c r="AI11" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="AK11" s="20" t="s">
-        <v>194</v>
-      </c>
-      <c r="AL11" s="21"/>
-      <c r="AM11" s="22"/>
-      <c r="AN11" s="23" t="s">
-        <v>210</v>
+      <c r="AK11" s="45" t="s">
+        <v>1360</v>
+      </c>
+      <c r="AL11" s="79"/>
+      <c r="AM11" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="AN11" s="45" t="s">
+        <v>101</v>
       </c>
       <c r="AO11" s="24"/>
       <c r="AP11" s="19" t="s">
@@ -9690,14 +9722,14 @@
       <c r="AI12" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="AK12" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="AL12" s="26" t="s">
-        <v>240</v>
-      </c>
-      <c r="AM12" s="27"/>
-      <c r="AN12" s="27"/>
+      <c r="AK12" s="7" t="s">
+        <v>1361</v>
+      </c>
+      <c r="AL12" s="79"/>
+      <c r="AM12" s="5"/>
+      <c r="AN12" s="5" t="s">
+        <v>1362</v>
+      </c>
       <c r="AO12" s="28"/>
       <c r="AP12" s="19" t="s">
         <v>241</v>
@@ -9773,12 +9805,10 @@
       <c r="AI13" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="AK13" s="22"/>
-      <c r="AL13" s="29" t="s">
-        <v>253</v>
-      </c>
-      <c r="AM13" s="22"/>
-      <c r="AN13" s="22"/>
+      <c r="AK13" s="79"/>
+      <c r="AL13" s="79"/>
+      <c r="AM13" s="79"/>
+      <c r="AN13" s="79"/>
       <c r="AO13" s="22"/>
       <c r="AP13" s="19" t="s">
         <v>261</v>
@@ -9849,12 +9879,14 @@
       <c r="AI14" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="AK14" s="31"/>
-      <c r="AL14" s="29" t="s">
-        <v>278</v>
-      </c>
+      <c r="AK14" s="65" t="s">
+        <v>194</v>
+      </c>
+      <c r="AL14" s="52"/>
       <c r="AM14" s="22"/>
-      <c r="AN14" s="22"/>
+      <c r="AN14" s="23" t="s">
+        <v>210</v>
+      </c>
       <c r="AO14" s="22"/>
       <c r="AP14" s="19" t="s">
         <v>279</v>
@@ -9914,12 +9946,14 @@
       <c r="AI15" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="AK15" s="31"/>
-      <c r="AL15" s="29" t="s">
-        <v>293</v>
-      </c>
-      <c r="AM15" s="31"/>
-      <c r="AN15" s="31"/>
+      <c r="AK15" s="49" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL15" s="58" t="s">
+        <v>240</v>
+      </c>
+      <c r="AM15" s="27"/>
+      <c r="AN15" s="27"/>
       <c r="AP15" s="19" t="s">
         <v>294</v>
       </c>
@@ -9987,14 +10021,12 @@
       <c r="AI16" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="AK16" s="32" t="s">
-        <v>310</v>
-      </c>
-      <c r="AL16" s="33" t="s">
-        <v>314</v>
-      </c>
-      <c r="AM16" s="34"/>
-      <c r="AN16" s="35"/>
+      <c r="AK16" s="79"/>
+      <c r="AL16" s="79" t="s">
+        <v>253</v>
+      </c>
+      <c r="AM16" s="22"/>
+      <c r="AN16" s="22"/>
       <c r="AP16" s="19" t="s">
         <v>315</v>
       </c>
@@ -10064,8 +10096,10 @@
       <c r="AI17" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="AK17" s="31"/>
-      <c r="AL17" s="22"/>
+      <c r="AK17" s="79"/>
+      <c r="AL17" s="79" t="s">
+        <v>278</v>
+      </c>
       <c r="AM17" s="22"/>
       <c r="AN17" s="22"/>
       <c r="AO17" s="22"/>
@@ -10132,14 +10166,12 @@
       <c r="AI18" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="AK18" s="37" t="s">
-        <v>343</v>
-      </c>
-      <c r="AL18" s="27"/>
-      <c r="AM18" s="27"/>
-      <c r="AN18" s="23" t="s">
-        <v>345</v>
-      </c>
+      <c r="AK18" s="79"/>
+      <c r="AL18" s="79" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM18" s="31"/>
+      <c r="AN18" s="31"/>
       <c r="AO18" s="31"/>
       <c r="AR18" s="3" t="s">
         <v>346</v>
@@ -10207,18 +10239,14 @@
       <c r="AE19" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="AK19" s="39" t="s">
-        <v>355</v>
-      </c>
-      <c r="AL19" s="40" t="s">
-        <v>363</v>
-      </c>
-      <c r="AM19" s="40" t="s">
-        <v>371</v>
-      </c>
-      <c r="AN19" s="40" t="s">
-        <v>373</v>
-      </c>
+      <c r="AK19" s="32" t="s">
+        <v>310</v>
+      </c>
+      <c r="AL19" s="33" t="s">
+        <v>314</v>
+      </c>
+      <c r="AM19" s="34"/>
+      <c r="AN19" s="35"/>
       <c r="AO19" s="24"/>
       <c r="AQ19" s="7" t="s">
         <v>375</v>
@@ -10288,18 +10316,10 @@
       <c r="AH20" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="AK20" s="41" t="s">
-        <v>343</v>
-      </c>
-      <c r="AL20" s="42" t="s">
-        <v>391</v>
-      </c>
-      <c r="AM20" s="42" t="s">
-        <v>392</v>
-      </c>
-      <c r="AN20" s="42" t="s">
-        <v>393</v>
-      </c>
+      <c r="AK20" s="31"/>
+      <c r="AL20" s="22"/>
+      <c r="AM20" s="22"/>
+      <c r="AN20" s="22"/>
       <c r="AO20" s="28"/>
       <c r="AQ20" s="7" t="s">
         <v>394</v>
@@ -10364,14 +10384,14 @@
       <c r="AI21" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="AK21" s="34"/>
-      <c r="AL21" s="42" t="s">
-        <v>407</v>
-      </c>
-      <c r="AM21" s="42" t="s">
-        <v>408</v>
-      </c>
-      <c r="AN21" s="43"/>
+      <c r="AK21" s="37" t="s">
+        <v>343</v>
+      </c>
+      <c r="AL21" s="27"/>
+      <c r="AM21" s="27"/>
+      <c r="AN21" s="23" t="s">
+        <v>345</v>
+      </c>
       <c r="AO21" s="31"/>
       <c r="AQ21" s="7" t="s">
         <v>409</v>
@@ -10439,10 +10459,18 @@
       <c r="AI22" s="4" t="s">
         <v>425</v>
       </c>
-      <c r="AK22" s="22"/>
-      <c r="AL22" s="31"/>
-      <c r="AM22" s="31"/>
-      <c r="AN22" s="31"/>
+      <c r="AK22" s="39" t="s">
+        <v>355</v>
+      </c>
+      <c r="AL22" s="40" t="s">
+        <v>363</v>
+      </c>
+      <c r="AM22" s="40" t="s">
+        <v>371</v>
+      </c>
+      <c r="AN22" s="40" t="s">
+        <v>373</v>
+      </c>
       <c r="AO22" s="31"/>
       <c r="AQ22" s="7" t="s">
         <v>422</v>
@@ -10511,13 +10539,17 @@
       <c r="AI23" s="4" t="s">
         <v>444</v>
       </c>
-      <c r="AK23" s="37" t="s">
-        <v>433</v>
-      </c>
-      <c r="AL23" s="27"/>
-      <c r="AM23" s="27"/>
-      <c r="AN23" s="23" t="s">
-        <v>435</v>
+      <c r="AK23" s="41" t="s">
+        <v>343</v>
+      </c>
+      <c r="AL23" s="42" t="s">
+        <v>391</v>
+      </c>
+      <c r="AM23" s="42" t="s">
+        <v>392</v>
+      </c>
+      <c r="AN23" s="42" t="s">
+        <v>393</v>
       </c>
       <c r="AO23" s="27"/>
       <c r="AQ23" s="7" t="s">
@@ -10577,13 +10609,13 @@
       <c r="AI24" s="4" t="s">
         <v>452</v>
       </c>
-      <c r="AK24" s="44" t="s">
-        <v>447</v>
-      </c>
-      <c r="AL24" s="33" t="s">
-        <v>453</v>
-      </c>
-      <c r="AM24" s="43"/>
+      <c r="AK24" s="34"/>
+      <c r="AL24" s="42" t="s">
+        <v>407</v>
+      </c>
+      <c r="AM24" s="42" t="s">
+        <v>408</v>
+      </c>
       <c r="AN24" s="43"/>
       <c r="AO24" s="24"/>
       <c r="AQ24" s="7" t="s">
@@ -10654,11 +10686,9 @@
         <v>467</v>
       </c>
       <c r="AK25" s="22"/>
-      <c r="AL25" s="33" t="s">
-        <v>468</v>
-      </c>
-      <c r="AM25" s="43"/>
-      <c r="AN25" s="43"/>
+      <c r="AL25" s="31"/>
+      <c r="AM25" s="31"/>
+      <c r="AN25" s="31"/>
       <c r="AO25" s="28"/>
       <c r="AQ25" s="7" t="s">
         <v>469</v>
@@ -10721,12 +10751,14 @@
       <c r="AI26" s="4" t="s">
         <v>483</v>
       </c>
-      <c r="AK26" s="22"/>
-      <c r="AL26" s="33" t="s">
-        <v>484</v>
-      </c>
-      <c r="AM26" s="46"/>
-      <c r="AN26" s="46"/>
+      <c r="AK26" s="37" t="s">
+        <v>433</v>
+      </c>
+      <c r="AL26" s="27"/>
+      <c r="AM26" s="27"/>
+      <c r="AN26" s="23" t="s">
+        <v>435</v>
+      </c>
       <c r="AO26" s="47"/>
       <c r="AQ26" s="7" t="s">
         <v>485</v>
@@ -10789,14 +10821,14 @@
       <c r="AI27" s="4" t="s">
         <v>500</v>
       </c>
-      <c r="AK27" s="39" t="s">
-        <v>501</v>
-      </c>
-      <c r="AL27" s="40" t="s">
-        <v>502</v>
-      </c>
-      <c r="AM27" s="21"/>
-      <c r="AN27" s="21"/>
+      <c r="AK27" s="44" t="s">
+        <v>447</v>
+      </c>
+      <c r="AL27" s="33" t="s">
+        <v>453</v>
+      </c>
+      <c r="AM27" s="43"/>
+      <c r="AN27" s="43"/>
       <c r="AO27" s="47"/>
       <c r="AP27" s="47"/>
     </row>
@@ -10846,14 +10878,12 @@
       <c r="AF28" s="4" t="s">
         <v>515</v>
       </c>
-      <c r="AK28" s="51"/>
-      <c r="AL28" s="40" t="s">
-        <v>516</v>
-      </c>
-      <c r="AM28" s="40" t="s">
-        <v>517</v>
-      </c>
-      <c r="AN28" s="52"/>
+      <c r="AK28" s="22"/>
+      <c r="AL28" s="33" t="s">
+        <v>468</v>
+      </c>
+      <c r="AM28" s="43"/>
+      <c r="AN28" s="43"/>
       <c r="AO28" s="22"/>
       <c r="AP28" s="3" t="s">
         <v>518</v>
@@ -10907,16 +10937,12 @@
       <c r="Z29" s="5"/>
       <c r="AA29" s="5"/>
       <c r="AB29" s="5"/>
-      <c r="AK29" s="44" t="s">
-        <v>533</v>
-      </c>
-      <c r="AL29" s="42" t="s">
-        <v>535</v>
-      </c>
-      <c r="AM29" s="33" t="s">
-        <v>536</v>
-      </c>
-      <c r="AN29" s="43"/>
+      <c r="AK29" s="22"/>
+      <c r="AL29" s="33" t="s">
+        <v>484</v>
+      </c>
+      <c r="AM29" s="46"/>
+      <c r="AN29" s="46"/>
       <c r="AO29" s="22"/>
       <c r="AP29" s="7" t="s">
         <v>534</v>
@@ -10950,16 +10976,14 @@
       <c r="P30" s="7" t="s">
         <v>538</v>
       </c>
-      <c r="AK30" s="44" t="s">
-        <v>540</v>
-      </c>
-      <c r="AL30" s="42" t="s">
-        <v>548</v>
-      </c>
-      <c r="AM30" s="33" t="s">
-        <v>549</v>
-      </c>
-      <c r="AN30" s="43"/>
+      <c r="AK30" s="39" t="s">
+        <v>501</v>
+      </c>
+      <c r="AL30" s="40" t="s">
+        <v>502</v>
+      </c>
+      <c r="AM30" s="21"/>
+      <c r="AN30" s="21"/>
       <c r="AO30" s="22"/>
       <c r="AP30" s="7" t="s">
         <v>544</v>
@@ -11021,16 +11045,14 @@
       <c r="AH31" s="3" t="s">
         <v>564</v>
       </c>
-      <c r="AK31" s="44" t="s">
-        <v>565</v>
-      </c>
-      <c r="AL31" s="42" t="s">
-        <v>568</v>
-      </c>
-      <c r="AM31" s="33" t="s">
-        <v>549</v>
-      </c>
-      <c r="AN31" s="46"/>
+      <c r="AK31" s="51"/>
+      <c r="AL31" s="40" t="s">
+        <v>516</v>
+      </c>
+      <c r="AM31" s="40" t="s">
+        <v>517</v>
+      </c>
+      <c r="AN31" s="52"/>
       <c r="AO31" s="22"/>
       <c r="AP31" s="7" t="s">
         <v>567</v>
@@ -11107,10 +11129,16 @@
       <c r="AI32" s="4" t="s">
         <v>596</v>
       </c>
-      <c r="AK32" s="31"/>
-      <c r="AL32" s="22"/>
-      <c r="AM32" s="22"/>
-      <c r="AN32" s="22"/>
+      <c r="AK32" s="44" t="s">
+        <v>533</v>
+      </c>
+      <c r="AL32" s="42" t="s">
+        <v>535</v>
+      </c>
+      <c r="AM32" s="33" t="s">
+        <v>536</v>
+      </c>
+      <c r="AN32" s="43"/>
       <c r="AO32" s="22"/>
       <c r="AP32" s="7" t="s">
         <v>582</v>
@@ -11171,14 +11199,16 @@
       <c r="AI33" s="4" t="s">
         <v>596</v>
       </c>
-      <c r="AK33" s="37" t="s">
-        <v>592</v>
-      </c>
-      <c r="AL33" s="58"/>
-      <c r="AM33" s="58"/>
-      <c r="AN33" s="23" t="s">
-        <v>601</v>
-      </c>
+      <c r="AK33" s="44" t="s">
+        <v>540</v>
+      </c>
+      <c r="AL33" s="42" t="s">
+        <v>548</v>
+      </c>
+      <c r="AM33" s="33" t="s">
+        <v>549</v>
+      </c>
+      <c r="AN33" s="43"/>
       <c r="AO33" s="24"/>
       <c r="AP33" s="24"/>
     </row>
@@ -11232,14 +11262,16 @@
       <c r="AI34" s="4" t="s">
         <v>620</v>
       </c>
-      <c r="AK34" s="59" t="s">
-        <v>447</v>
-      </c>
-      <c r="AL34" s="33" t="s">
-        <v>621</v>
-      </c>
-      <c r="AM34" s="43"/>
-      <c r="AN34" s="43"/>
+      <c r="AK34" s="44" t="s">
+        <v>565</v>
+      </c>
+      <c r="AL34" s="42" t="s">
+        <v>568</v>
+      </c>
+      <c r="AM34" s="33" t="s">
+        <v>549</v>
+      </c>
+      <c r="AN34" s="46"/>
       <c r="AO34" s="28"/>
       <c r="AP34" s="60" t="s">
         <v>622</v>
@@ -11289,14 +11321,10 @@
       <c r="AI35" s="4" t="s">
         <v>638</v>
       </c>
-      <c r="AK35" s="61"/>
-      <c r="AL35" s="33" t="s">
-        <v>639</v>
-      </c>
-      <c r="AM35" s="42" t="s">
-        <v>640</v>
-      </c>
-      <c r="AN35" s="43"/>
+      <c r="AK35" s="31"/>
+      <c r="AL35" s="22"/>
+      <c r="AM35" s="22"/>
+      <c r="AN35" s="22"/>
       <c r="AO35" s="22"/>
       <c r="AP35" s="18" t="s">
         <v>641</v>
@@ -11363,10 +11391,14 @@
       <c r="AF36" s="3" t="s">
         <v>658</v>
       </c>
-      <c r="AK36" s="22"/>
-      <c r="AL36" s="22"/>
-      <c r="AM36" s="22"/>
-      <c r="AN36" s="22"/>
+      <c r="AK36" s="37" t="s">
+        <v>592</v>
+      </c>
+      <c r="AL36" s="58"/>
+      <c r="AM36" s="58"/>
+      <c r="AN36" s="23" t="s">
+        <v>601</v>
+      </c>
       <c r="AO36" s="22"/>
       <c r="AP36" s="18" t="s">
         <v>661</v>
@@ -11440,14 +11472,14 @@
       <c r="AH37" s="3" t="s">
         <v>670</v>
       </c>
-      <c r="AK37" s="37" t="s">
-        <v>672</v>
-      </c>
-      <c r="AL37" s="58"/>
-      <c r="AM37" s="58"/>
-      <c r="AN37" s="23" t="s">
-        <v>435</v>
-      </c>
+      <c r="AK37" s="59" t="s">
+        <v>447</v>
+      </c>
+      <c r="AL37" s="33" t="s">
+        <v>621</v>
+      </c>
+      <c r="AM37" s="43"/>
+      <c r="AN37" s="43"/>
       <c r="AO37" s="24"/>
       <c r="AP37" s="29"/>
       <c r="AS37" s="7" t="s">
@@ -11517,14 +11549,14 @@
       <c r="AI38" s="4" t="s">
         <v>696</v>
       </c>
-      <c r="AK38" s="24" t="s">
-        <v>14</v>
-      </c>
+      <c r="AK38" s="61"/>
       <c r="AL38" s="33" t="s">
-        <v>697</v>
-      </c>
-      <c r="AM38" s="46"/>
-      <c r="AN38" s="46"/>
+        <v>639</v>
+      </c>
+      <c r="AM38" s="42" t="s">
+        <v>640</v>
+      </c>
+      <c r="AN38" s="43"/>
       <c r="AO38" s="64"/>
       <c r="AP38" s="29"/>
       <c r="AS38" s="7" t="s">
@@ -11582,12 +11614,10 @@
       <c r="AI39" s="4" t="s">
         <v>712</v>
       </c>
-      <c r="AK39" s="65"/>
-      <c r="AL39" s="33" t="s">
-        <v>713</v>
-      </c>
-      <c r="AM39" s="46"/>
-      <c r="AN39" s="46"/>
+      <c r="AK39" s="22"/>
+      <c r="AL39" s="22"/>
+      <c r="AM39" s="22"/>
+      <c r="AN39" s="22"/>
       <c r="AO39" s="22"/>
       <c r="AP39" s="22"/>
       <c r="AS39" s="7" t="s">
@@ -11628,12 +11658,14 @@
       <c r="AI40" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="AK40" s="65"/>
-      <c r="AL40" s="33" t="s">
-        <v>727</v>
-      </c>
-      <c r="AM40" s="46"/>
-      <c r="AN40" s="46"/>
+      <c r="AK40" s="37" t="s">
+        <v>672</v>
+      </c>
+      <c r="AL40" s="58"/>
+      <c r="AM40" s="58"/>
+      <c r="AN40" s="23" t="s">
+        <v>435</v>
+      </c>
       <c r="AO40" s="22"/>
       <c r="AP40" s="22"/>
       <c r="AS40" s="7" t="s">
@@ -11696,14 +11728,14 @@
       <c r="AI41" s="4" t="s">
         <v>745</v>
       </c>
-      <c r="AK41" s="26" t="s">
-        <v>737</v>
-      </c>
-      <c r="AL41" s="26" t="s">
-        <v>738</v>
-      </c>
-      <c r="AM41" s="65"/>
-      <c r="AN41" s="65"/>
+      <c r="AK41" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL41" s="33" t="s">
+        <v>697</v>
+      </c>
+      <c r="AM41" s="46"/>
+      <c r="AN41" s="46"/>
       <c r="AO41" s="22"/>
       <c r="AS41" s="7" t="s">
         <v>746</v>
@@ -11762,18 +11794,12 @@
       <c r="AI42" s="4" t="s">
         <v>765</v>
       </c>
-      <c r="AK42" s="67">
-        <v>0</v>
-      </c>
-      <c r="AL42" s="29" t="s">
-        <v>743</v>
-      </c>
-      <c r="AM42" s="33" t="s">
-        <v>767</v>
-      </c>
-      <c r="AN42" s="33" t="s">
-        <v>768</v>
-      </c>
+      <c r="AK42" s="65"/>
+      <c r="AL42" s="33" t="s">
+        <v>713</v>
+      </c>
+      <c r="AM42" s="46"/>
+      <c r="AN42" s="46"/>
       <c r="AO42" s="22"/>
       <c r="AS42" s="7" t="s">
         <v>769</v>
@@ -11831,16 +11857,12 @@
       <c r="AI43" s="4" t="s">
         <v>781</v>
       </c>
-      <c r="AK43" s="22"/>
-      <c r="AL43" s="29" t="s">
-        <v>755</v>
-      </c>
-      <c r="AM43" s="33" t="s">
-        <v>782</v>
-      </c>
-      <c r="AN43" s="33" t="s">
-        <v>783</v>
-      </c>
+      <c r="AK43" s="65"/>
+      <c r="AL43" s="33" t="s">
+        <v>727</v>
+      </c>
+      <c r="AM43" s="46"/>
+      <c r="AN43" s="46"/>
       <c r="AO43" s="22"/>
       <c r="AT43" s="63" t="s">
         <v>784</v>
@@ -11901,10 +11923,14 @@
       <c r="AI44" s="4" t="s">
         <v>794</v>
       </c>
-      <c r="AK44" s="69"/>
-      <c r="AL44" s="69"/>
-      <c r="AM44" s="69"/>
-      <c r="AN44" s="69"/>
+      <c r="AK44" s="26" t="s">
+        <v>737</v>
+      </c>
+      <c r="AL44" s="26" t="s">
+        <v>738</v>
+      </c>
+      <c r="AM44" s="65"/>
+      <c r="AN44" s="65"/>
       <c r="AO44" s="69"/>
       <c r="AR44" s="3" t="s">
         <v>795</v>
@@ -11964,6 +11990,22 @@
         <v>808</v>
       </c>
       <c r="AF45" s="3"/>
+      <c r="AK45" s="67">
+        <v>0</v>
+      </c>
+      <c r="AL45" s="29" t="s">
+        <v>743</v>
+      </c>
+      <c r="AM45" s="33" t="s">
+        <v>767</v>
+      </c>
+      <c r="AN45" s="33" t="s">
+        <v>768</v>
+      </c>
+      <c r="AO45" s="3" t="s">
+        <v>848</v>
+      </c>
+      <c r="AP45" s="53"/>
       <c r="AR45" s="4" t="s">
         <v>810</v>
       </c>
@@ -12015,6 +12057,22 @@
       <c r="AI46" s="3" t="s">
         <v>826</v>
       </c>
+      <c r="AK46" s="22"/>
+      <c r="AL46" s="29" t="s">
+        <v>755</v>
+      </c>
+      <c r="AM46" s="33" t="s">
+        <v>782</v>
+      </c>
+      <c r="AN46" s="33" t="s">
+        <v>783</v>
+      </c>
+      <c r="AO46" s="3" t="s">
+        <v>866</v>
+      </c>
+      <c r="AP46" s="3" t="s">
+        <v>867</v>
+      </c>
       <c r="AR46" s="4" t="s">
         <v>827</v>
       </c>
@@ -12067,6 +12125,16 @@
       <c r="AI47" s="70" t="s">
         <v>849</v>
       </c>
+      <c r="AK47" s="69"/>
+      <c r="AL47" s="69"/>
+      <c r="AM47" s="69"/>
+      <c r="AN47" s="69"/>
+      <c r="AO47" s="70" t="s">
+        <v>895</v>
+      </c>
+      <c r="AP47" s="70" t="s">
+        <v>896</v>
+      </c>
       <c r="AR47" s="4" t="s">
         <v>851</v>
       </c>
@@ -12116,13 +12184,12 @@
       <c r="AI48" s="70" t="s">
         <v>861</v>
       </c>
-      <c r="AL48" s="3" t="s">
-        <v>850</v>
-      </c>
-      <c r="AN48" s="3" t="s">
-        <v>848</v>
-      </c>
-      <c r="AO48" s="53"/>
+      <c r="AO48" s="70" t="s">
+        <v>909</v>
+      </c>
+      <c r="AP48" s="70" t="s">
+        <v>910</v>
+      </c>
       <c r="AR48" s="4" t="s">
         <v>862</v>
       </c>
@@ -12164,14 +12231,11 @@
       <c r="AI49" s="70" t="s">
         <v>874</v>
       </c>
-      <c r="AL49" s="3" t="s">
-        <v>864</v>
-      </c>
-      <c r="AN49" s="3" t="s">
-        <v>866</v>
-      </c>
-      <c r="AO49" s="3" t="s">
-        <v>867</v>
+      <c r="AO49" s="70" t="s">
+        <v>925</v>
+      </c>
+      <c r="AP49" s="70" t="s">
+        <v>926</v>
       </c>
     </row>
     <row r="50" spans="1:46" ht="14.25" customHeight="1">
@@ -12221,14 +12285,11 @@
       <c r="AI50" s="70" t="s">
         <v>892</v>
       </c>
-      <c r="AL50" s="4" t="s">
-        <v>893</v>
-      </c>
-      <c r="AN50" s="70" t="s">
-        <v>895</v>
-      </c>
       <c r="AO50" s="70" t="s">
-        <v>896</v>
+        <v>947</v>
+      </c>
+      <c r="AP50" s="70" t="s">
+        <v>948</v>
       </c>
       <c r="AR50" s="3" t="s">
         <v>880</v>
@@ -12287,14 +12348,14 @@
       <c r="AI51" s="70" t="s">
         <v>907</v>
       </c>
-      <c r="AL51" s="4" t="s">
-        <v>908</v>
-      </c>
-      <c r="AN51" s="70" t="s">
-        <v>909</v>
+      <c r="AL51" s="3" t="s">
+        <v>850</v>
       </c>
       <c r="AO51" s="70" t="s">
-        <v>910</v>
+        <v>971</v>
+      </c>
+      <c r="AP51" s="70" t="s">
+        <v>972</v>
       </c>
       <c r="AR51" s="4" t="s">
         <v>911</v>
@@ -12343,14 +12404,14 @@
       <c r="AD52" s="7" t="s">
         <v>923</v>
       </c>
-      <c r="AL52" s="4" t="s">
-        <v>924</v>
-      </c>
-      <c r="AN52" s="70" t="s">
-        <v>925</v>
+      <c r="AL52" s="3" t="s">
+        <v>864</v>
       </c>
       <c r="AO52" s="70" t="s">
-        <v>926</v>
+        <v>981</v>
+      </c>
+      <c r="AP52" s="70" t="s">
+        <v>982</v>
       </c>
       <c r="AR52" s="4" t="s">
         <v>928</v>
@@ -12417,13 +12478,7 @@
         <v>945</v>
       </c>
       <c r="AL53" s="4" t="s">
-        <v>946</v>
-      </c>
-      <c r="AN53" s="70" t="s">
-        <v>947</v>
-      </c>
-      <c r="AO53" s="70" t="s">
-        <v>948</v>
+        <v>893</v>
       </c>
       <c r="AR53" s="4" t="s">
         <v>950</v>
@@ -12488,13 +12543,7 @@
         <v>967</v>
       </c>
       <c r="AL54" s="4" t="s">
-        <v>970</v>
-      </c>
-      <c r="AN54" s="70" t="s">
-        <v>971</v>
-      </c>
-      <c r="AO54" s="70" t="s">
-        <v>972</v>
+        <v>908</v>
       </c>
     </row>
     <row r="55" spans="1:46" ht="14.25" customHeight="1">
@@ -12547,13 +12596,7 @@
         <v>979</v>
       </c>
       <c r="AL55" s="4" t="s">
-        <v>980</v>
-      </c>
-      <c r="AN55" s="70" t="s">
-        <v>981</v>
-      </c>
-      <c r="AO55" s="70" t="s">
-        <v>982</v>
+        <v>924</v>
       </c>
       <c r="AR55" s="56" t="s">
         <v>949</v>
@@ -12607,7 +12650,7 @@
         <v>992</v>
       </c>
       <c r="AL56" s="4" t="s">
-        <v>993</v>
+        <v>946</v>
       </c>
       <c r="AR56" s="3" t="s">
         <v>957</v>
@@ -12665,7 +12708,7 @@
       </c>
       <c r="X57" s="5"/>
       <c r="AL57" s="4" t="s">
-        <v>998</v>
+        <v>970</v>
       </c>
       <c r="AQ57" s="7" t="s">
         <v>973</v>
@@ -12720,7 +12763,7 @@
         <v>922</v>
       </c>
       <c r="AL58" s="4" t="s">
-        <v>1010</v>
+        <v>980</v>
       </c>
       <c r="AQ58" s="7" t="s">
         <v>995</v>
@@ -12782,8 +12825,8 @@
         <v>1029</v>
       </c>
       <c r="AE59" s="4"/>
-      <c r="AL59" s="3" t="s">
-        <v>1006</v>
+      <c r="AL59" s="4" t="s">
+        <v>993</v>
       </c>
       <c r="AQ59" s="7" t="s">
         <v>1008</v>
@@ -12846,7 +12889,7 @@
       </c>
       <c r="AE60" s="4"/>
       <c r="AL60" s="4" t="s">
-        <v>970</v>
+        <v>998</v>
       </c>
     </row>
     <row r="61" spans="1:46" ht="14.25" customHeight="1">
@@ -12895,7 +12938,7 @@
       <c r="Z61" s="5"/>
       <c r="AA61" s="5"/>
       <c r="AL61" s="4" t="s">
-        <v>1059</v>
+        <v>1010</v>
       </c>
       <c r="AS61" s="7"/>
       <c r="AT61" s="3" t="s">
@@ -12947,8 +12990,8 @@
       </c>
       <c r="Z62" s="4"/>
       <c r="AA62" s="4"/>
-      <c r="AL62" s="4" t="s">
-        <v>1070</v>
+      <c r="AL62" s="3" t="s">
+        <v>1006</v>
       </c>
       <c r="AS62" s="7" t="s">
         <v>1071</v>
@@ -12996,7 +13039,7 @@
         <v>1080</v>
       </c>
       <c r="AL63" s="4" t="s">
-        <v>1081</v>
+        <v>970</v>
       </c>
       <c r="AS63" s="7" t="s">
         <v>1082</v>
@@ -13037,8 +13080,9 @@
       <c r="AD64" s="7" t="s">
         <v>1103</v>
       </c>
-      <c r="AL64" s="3"/>
-      <c r="AN64" s="3"/>
+      <c r="AL64" s="4" t="s">
+        <v>1059</v>
+      </c>
       <c r="AS64" s="7" t="s">
         <v>1105</v>
       </c>
@@ -13075,11 +13119,8 @@
       <c r="AD65" s="7" t="s">
         <v>1124</v>
       </c>
-      <c r="AL65" s="3" t="s">
-        <v>1053</v>
-      </c>
-      <c r="AN65" s="3" t="s">
-        <v>1054</v>
+      <c r="AL65" s="4" t="s">
+        <v>1070</v>
       </c>
       <c r="AO65" s="3" t="s">
         <v>1126</v>
@@ -13138,10 +13179,7 @@
         <v>115</v>
       </c>
       <c r="AL66" s="4" t="s">
-        <v>1141</v>
-      </c>
-      <c r="AN66" s="7" t="s">
-        <v>1060</v>
+        <v>1081</v>
       </c>
       <c r="AO66" s="70" t="s">
         <v>1142</v>
@@ -13203,12 +13241,8 @@
       <c r="AD67" s="7" t="s">
         <v>1151</v>
       </c>
-      <c r="AL67" s="4" t="s">
-        <v>1152</v>
-      </c>
-      <c r="AN67" s="7" t="s">
-        <v>1073</v>
-      </c>
+      <c r="AL67" s="3"/>
+      <c r="AN67" s="3"/>
       <c r="AO67" s="70" t="s">
         <v>1153</v>
       </c>
@@ -13275,11 +13309,11 @@
       <c r="AD68" s="7" t="s">
         <v>1166</v>
       </c>
-      <c r="AL68" s="4" t="s">
-        <v>970</v>
-      </c>
-      <c r="AN68" s="7" t="s">
-        <v>1089</v>
+      <c r="AL68" s="3" t="s">
+        <v>1053</v>
+      </c>
+      <c r="AN68" s="3" t="s">
+        <v>1054</v>
       </c>
       <c r="AO68" s="70" t="s">
         <v>1167</v>
@@ -13345,7 +13379,10 @@
         <v>115</v>
       </c>
       <c r="AL69" s="4" t="s">
-        <v>1179</v>
+        <v>1141</v>
+      </c>
+      <c r="AN69" s="7" t="s">
+        <v>1060</v>
       </c>
       <c r="AS69" s="7" t="s">
         <v>1180</v>
@@ -13397,6 +13434,12 @@
       <c r="AD70" s="7" t="s">
         <v>1151</v>
       </c>
+      <c r="AL70" s="4" t="s">
+        <v>1152</v>
+      </c>
+      <c r="AN70" s="7" t="s">
+        <v>1073</v>
+      </c>
       <c r="AS70" s="7" t="s">
         <v>1188</v>
       </c>
@@ -13435,6 +13478,12 @@
       <c r="Z71" s="78" t="s">
         <v>50</v>
       </c>
+      <c r="AL71" s="4" t="s">
+        <v>970</v>
+      </c>
+      <c r="AN71" s="7" t="s">
+        <v>1089</v>
+      </c>
     </row>
     <row r="72" spans="1:47" ht="14.25" customHeight="1">
       <c r="A72" s="18" t="s">
@@ -13470,8 +13519,8 @@
       <c r="Z72" s="77" t="s">
         <v>50</v>
       </c>
-      <c r="AN72" s="3" t="s">
-        <v>1098</v>
+      <c r="AL72" s="4" t="s">
+        <v>1179</v>
       </c>
       <c r="AO72" s="3" t="s">
         <v>1099</v>
@@ -13524,9 +13573,6 @@
       <c r="X73" s="19" t="s">
         <v>1204</v>
       </c>
-      <c r="AN73" s="7" t="s">
-        <v>1107</v>
-      </c>
       <c r="AO73" s="70" t="s">
         <v>1205</v>
       </c>
@@ -13583,9 +13629,6 @@
       <c r="X74" s="19" t="s">
         <v>1212</v>
       </c>
-      <c r="AN74" s="7" t="s">
-        <v>1111</v>
-      </c>
       <c r="AO74" s="70" t="s">
         <v>1213</v>
       </c>
@@ -13630,8 +13673,8 @@
       <c r="V75" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="AN75" s="7" t="s">
-        <v>1114</v>
+      <c r="AN75" s="3" t="s">
+        <v>1098</v>
       </c>
       <c r="AO75" s="70" t="s">
         <v>1216</v>
@@ -13687,7 +13730,7 @@
         <v>50</v>
       </c>
       <c r="AN76" s="7" t="s">
-        <v>1118</v>
+        <v>1107</v>
       </c>
       <c r="AO76" s="70" t="s">
         <v>1221</v>
@@ -13746,7 +13789,7 @@
         <v>115</v>
       </c>
       <c r="AN77" s="7" t="s">
-        <v>1122</v>
+        <v>1111</v>
       </c>
       <c r="AO77" s="70" t="s">
         <v>1229</v>
@@ -13804,6 +13847,9 @@
       <c r="V78" s="5" t="s">
         <v>50</v>
       </c>
+      <c r="AN78" s="7" t="s">
+        <v>1114</v>
+      </c>
       <c r="AS78" s="18" t="s">
         <v>115</v>
       </c>
@@ -13846,6 +13892,9 @@
       <c r="V79" s="5" t="s">
         <v>50</v>
       </c>
+      <c r="AN79" s="7" t="s">
+        <v>1118</v>
+      </c>
       <c r="AS79" s="18" t="s">
         <v>115</v>
       </c>
@@ -13868,6 +13917,9 @@
       </c>
       <c r="N80" s="56" t="s">
         <v>1110</v>
+      </c>
+      <c r="AN80" s="7" t="s">
+        <v>1122</v>
       </c>
     </row>
     <row r="81" spans="1:24" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
added bgp configuration order commit, updated drills
</commit_message>
<xml_diff>
--- a/written-exam-memory-drills.xlsx
+++ b/written-exam-memory-drills.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qdd/Google Drive/git/notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E533C92-4A12-F64C-B8BB-E87F1331FC0A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68ACB82F-9E61-7B47-9C34-D0B4C34FECFD}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5120" yWindow="460" windowWidth="30260" windowHeight="19960" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4377,7 +4377,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4493,6 +4493,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -8806,8 +8807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AU997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P74" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="S92" sqref="S92"/>
+    <sheetView tabSelected="1" topLeftCell="X19" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="Z32" sqref="Z32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9122,10 +9123,10 @@
       <c r="AS3" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="AT3" s="80" t="s">
+      <c r="AT3" s="81" t="s">
         <v>82</v>
       </c>
-      <c r="AU3" s="81"/>
+      <c r="AU3" s="82"/>
     </row>
     <row r="4" spans="1:47" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
@@ -9202,10 +9203,10 @@
       <c r="AQ4" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="AS4" s="80" t="s">
+      <c r="AS4" s="81" t="s">
         <v>116</v>
       </c>
-      <c r="AT4" s="81"/>
+      <c r="AT4" s="82"/>
       <c r="AU4" s="14"/>
     </row>
     <row r="5" spans="1:47" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -9254,10 +9255,10 @@
       <c r="AS5" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="AT5" s="80" t="s">
+      <c r="AT5" s="81" t="s">
         <v>128</v>
       </c>
-      <c r="AU5" s="81"/>
+      <c r="AU5" s="82"/>
     </row>
     <row r="6" spans="1:47" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
@@ -12118,7 +12119,8 @@
       <c r="U46" s="4" t="s">
         <v>820</v>
       </c>
-      <c r="Y46" s="4"/>
+      <c r="Y46" s="80"/>
+      <c r="Z46" s="80"/>
       <c r="AG46" s="3" t="s">
         <v>825</v>
       </c>
@@ -12180,7 +12182,8 @@
       <c r="W47" s="3" t="s">
         <v>809</v>
       </c>
-      <c r="Y47" s="5"/>
+      <c r="Y47" s="80"/>
+      <c r="Z47" s="80"/>
       <c r="AB47" s="3" t="s">
         <v>839</v>
       </c>
@@ -12239,7 +12242,8 @@
       <c r="X48" s="4" t="s">
         <v>857</v>
       </c>
-      <c r="Y48" s="5"/>
+      <c r="Y48" s="80"/>
+      <c r="Z48" s="80"/>
       <c r="AB48" s="70" t="s">
         <v>859</v>
       </c>
@@ -12286,7 +12290,8 @@
       <c r="X49" s="5" t="s">
         <v>869</v>
       </c>
-      <c r="Y49" s="4"/>
+      <c r="Y49" s="80"/>
+      <c r="Z49" s="80"/>
       <c r="AB49" s="11" t="s">
         <v>871</v>
       </c>
@@ -12341,6 +12346,8 @@
       <c r="X50" s="5" t="s">
         <v>887</v>
       </c>
+      <c r="Y50" s="80"/>
+      <c r="Z50" s="80"/>
       <c r="AB50" s="70" t="s">
         <v>889</v>
       </c>
@@ -12404,6 +12411,8 @@
       <c r="X51" s="4" t="s">
         <v>904</v>
       </c>
+      <c r="Y51" s="80"/>
+      <c r="Z51" s="80"/>
       <c r="AB51" s="11" t="s">
         <v>905</v>
       </c>
@@ -12461,8 +12470,8 @@
         <v>921</v>
       </c>
       <c r="V52" s="17"/>
-      <c r="Y52" s="4"/>
-      <c r="Z52" s="4"/>
+      <c r="Y52" s="80"/>
+      <c r="Z52" s="80"/>
       <c r="AB52" s="70" t="s">
         <v>50</v>
       </c>
@@ -12534,8 +12543,8 @@
       <c r="W53" s="3" t="s">
         <v>894</v>
       </c>
-      <c r="Y53" s="5"/>
-      <c r="Z53" s="5"/>
+      <c r="Y53" s="80"/>
+      <c r="Z53" s="80"/>
       <c r="AB53" s="11" t="s">
         <v>50</v>
       </c>
@@ -12599,8 +12608,8 @@
         <v>962</v>
       </c>
       <c r="X54" s="4"/>
-      <c r="Y54" s="4"/>
-      <c r="Z54" s="4"/>
+      <c r="Y54" s="80"/>
+      <c r="Z54" s="80"/>
       <c r="AB54" s="70" t="s">
         <v>964</v>
       </c>
@@ -12652,8 +12661,8 @@
         <v>978</v>
       </c>
       <c r="X55" s="5"/>
-      <c r="Y55" s="5"/>
-      <c r="Z55" s="5"/>
+      <c r="Y55" s="80"/>
+      <c r="Z55" s="80"/>
       <c r="AB55" s="11" t="s">
         <v>115</v>
       </c>
@@ -12706,8 +12715,8 @@
         <v>991</v>
       </c>
       <c r="X56" s="4"/>
-      <c r="Y56" s="5"/>
-      <c r="Z56" s="5"/>
+      <c r="Y56" s="80"/>
+      <c r="Z56" s="80"/>
       <c r="AB56" s="11" t="s">
         <v>50</v>
       </c>
@@ -12824,9 +12833,6 @@
         <v>1009</v>
       </c>
       <c r="X58" s="5"/>
-      <c r="Y58" s="3" t="s">
-        <v>660</v>
-      </c>
       <c r="AC58" s="3" t="s">
         <v>922</v>
       </c>
@@ -12881,11 +12887,6 @@
       <c r="U59" s="4" t="s">
         <v>1027</v>
       </c>
-      <c r="Y59" s="4" t="s">
-        <v>1028</v>
-      </c>
-      <c r="Z59" s="4"/>
-      <c r="AA59" s="4"/>
       <c r="AC59" s="7" t="s">
         <v>936</v>
       </c>
@@ -12944,11 +12945,9 @@
       <c r="X60" s="3" t="s">
         <v>987</v>
       </c>
-      <c r="Y60" s="5" t="s">
-        <v>1042</v>
-      </c>
-      <c r="Z60" s="5"/>
-      <c r="AA60" s="5"/>
+      <c r="Y60" s="3" t="s">
+        <v>660</v>
+      </c>
       <c r="AC60" s="7" t="s">
         <v>944</v>
       </c>
@@ -13000,11 +12999,11 @@
       <c r="X61" s="4" t="s">
         <v>1056</v>
       </c>
-      <c r="Y61" s="5" t="s">
-        <v>1058</v>
-      </c>
-      <c r="Z61" s="5"/>
-      <c r="AA61" s="5"/>
+      <c r="Y61" s="4" t="s">
+        <v>1028</v>
+      </c>
+      <c r="Z61" s="4"/>
+      <c r="AA61" s="4"/>
       <c r="AL61" s="4" t="s">
         <v>1010</v>
       </c>
@@ -13053,11 +13052,11 @@
       <c r="X62" s="5" t="s">
         <v>1068</v>
       </c>
-      <c r="Y62" s="4" t="s">
-        <v>1069</v>
-      </c>
-      <c r="Z62" s="4"/>
-      <c r="AA62" s="4"/>
+      <c r="Y62" s="5" t="s">
+        <v>1042</v>
+      </c>
+      <c r="Z62" s="5"/>
+      <c r="AA62" s="5"/>
       <c r="AL62" s="3" t="s">
         <v>1006</v>
       </c>
@@ -13106,6 +13105,11 @@
       <c r="X63" s="5" t="s">
         <v>1080</v>
       </c>
+      <c r="Y63" s="5" t="s">
+        <v>1058</v>
+      </c>
+      <c r="Z63" s="5"/>
+      <c r="AA63" s="5"/>
       <c r="AL63" s="4" t="s">
         <v>970</v>
       </c>
@@ -13136,12 +13140,11 @@
       <c r="X64" s="4" t="s">
         <v>1087</v>
       </c>
-      <c r="Y64" s="76" t="s">
-        <v>1088</v>
-      </c>
-      <c r="Z64" s="76" t="s">
-        <v>1094</v>
-      </c>
+      <c r="Y64" s="4" t="s">
+        <v>1069</v>
+      </c>
+      <c r="Z64" s="4"/>
+      <c r="AA64" s="4"/>
       <c r="AC64" s="7" t="s">
         <v>1100</v>
       </c>
@@ -13172,12 +13175,6 @@
         <v>1109</v>
       </c>
       <c r="L65" s="62"/>
-      <c r="Y65" s="77" t="s">
-        <v>115</v>
-      </c>
-      <c r="Z65" s="77" t="s">
-        <v>50</v>
-      </c>
       <c r="AB65" s="7" t="s">
         <v>1121</v>
       </c>
@@ -13234,12 +13231,6 @@
       <c r="V66" s="76">
         <v>3</v>
       </c>
-      <c r="Y66" s="78" t="s">
-        <v>115</v>
-      </c>
-      <c r="Z66" s="78" t="s">
-        <v>50</v>
-      </c>
       <c r="AB66" s="7" t="s">
         <v>1140</v>
       </c>
@@ -13300,11 +13291,11 @@
       <c r="X67" s="19" t="s">
         <v>1149</v>
       </c>
-      <c r="Y67" s="78" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z67" s="78" t="s">
-        <v>115</v>
+      <c r="Y67" s="76" t="s">
+        <v>1088</v>
+      </c>
+      <c r="Z67" s="76" t="s">
+        <v>1094</v>
       </c>
       <c r="AB67" s="7" t="s">
         <v>1150</v>
@@ -13439,10 +13430,10 @@
       <c r="X69" s="19" t="s">
         <v>1177</v>
       </c>
-      <c r="Y69" s="77" t="s">
+      <c r="Y69" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="Z69" s="77" t="s">
+      <c r="Z69" s="78" t="s">
         <v>50</v>
       </c>
       <c r="AB69" s="7" t="s">
@@ -13493,10 +13484,10 @@
         <v>103</v>
       </c>
       <c r="Y70" s="78" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z70" s="78" t="s">
         <v>115</v>
-      </c>
-      <c r="Z70" s="78" t="s">
-        <v>50</v>
       </c>
       <c r="AB70" s="7" t="s">
         <v>1187</v>
@@ -13554,10 +13545,10 @@
       <c r="X71" s="19" t="s">
         <v>1192</v>
       </c>
-      <c r="Y71" s="78" t="s">
+      <c r="Y71" s="77" t="s">
         <v>115</v>
       </c>
-      <c r="Z71" s="78" t="s">
+      <c r="Z71" s="77" t="s">
         <v>50</v>
       </c>
       <c r="AL71" s="4" t="s">
@@ -13667,6 +13658,12 @@
       <c r="X73" s="19" t="s">
         <v>1204</v>
       </c>
+      <c r="Y73" s="78" t="s">
+        <v>115</v>
+      </c>
+      <c r="Z73" s="78" t="s">
+        <v>50</v>
+      </c>
       <c r="AN73" s="7" t="s">
         <v>1114</v>
       </c>
@@ -13726,6 +13723,12 @@
       <c r="X74" s="19" t="s">
         <v>1212</v>
       </c>
+      <c r="Y74" s="78" t="s">
+        <v>115</v>
+      </c>
+      <c r="Z74" s="78" t="s">
+        <v>50</v>
+      </c>
       <c r="AN74" s="7" t="s">
         <v>1118</v>
       </c>
@@ -13771,6 +13774,12 @@
         <v>115</v>
       </c>
       <c r="V75" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y75" s="77" t="s">
+        <v>115</v>
+      </c>
+      <c r="Z75" s="77" t="s">
         <v>50</v>
       </c>
       <c r="AN75" s="7" t="s">

</xml_diff>

<commit_message>
added mindmap for dmvpn
</commit_message>
<xml_diff>
--- a/written-exam-memory-drills.xlsx
+++ b/written-exam-memory-drills.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qdd/Google Drive/git/notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEA939F0-2017-FA40-B522-BA28A659CD3C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5704AD4-D7E2-7940-80AF-89DF02D2CE3B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14680" yWindow="1220" windowWidth="21260" windowHeight="19960" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13320" yWindow="740" windowWidth="21260" windowHeight="19960" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fill-in" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2178" uniqueCount="1402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2178" uniqueCount="1403">
   <si>
     <t>bgp best-path</t>
   </si>
@@ -3532,9 +3532,6 @@
     <t>mac flooding</t>
   </si>
   <si>
-    <t>dynamic spoke-to-spoke</t>
-  </si>
-  <si>
     <t>vtp primary server</t>
   </si>
   <si>
@@ -4292,6 +4289,12 @@
   </si>
   <si>
     <t>Multicast</t>
+  </si>
+  <si>
+    <t>dynamic spoke-to-spoke tunneling</t>
+  </si>
+  <si>
+    <t>depends on routing protocol</t>
   </si>
 </sst>
 </file>
@@ -8888,8 +8891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AU997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ24" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="AN45" sqref="AN45"/>
+    <sheetView tabSelected="1" topLeftCell="S60" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="S68" sqref="S68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9790,7 +9793,7 @@
         <v>220</v>
       </c>
       <c r="AK11" s="45" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="AL11" s="79"/>
       <c r="AM11" s="45" t="s">
@@ -9872,12 +9875,12 @@
         <v>239</v>
       </c>
       <c r="AK12" s="7" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="AL12" s="79"/>
       <c r="AM12" s="5"/>
       <c r="AN12" s="5" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="AO12" s="28"/>
       <c r="AP12" s="19" t="s">
@@ -13357,12 +13360,12 @@
         <v>935</v>
       </c>
       <c r="K67" s="7" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="L67" s="7"/>
       <c r="M67" s="81"/>
       <c r="S67" s="7" t="s">
-        <v>1148</v>
+        <v>1401</v>
       </c>
       <c r="T67" s="5" t="s">
         <v>115</v>
@@ -13374,7 +13377,7 @@
         <v>50</v>
       </c>
       <c r="X67" s="19" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="Y67" s="76" t="s">
         <v>1088</v>
@@ -13383,30 +13386,30 @@
         <v>1094</v>
       </c>
       <c r="AB67" s="7" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="AC67" s="7" t="s">
         <v>50</v>
       </c>
       <c r="AD67" s="7" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="AL67" s="3"/>
       <c r="AN67" s="7" t="s">
         <v>1073</v>
       </c>
       <c r="AO67" s="70" t="s">
+        <v>1152</v>
+      </c>
+      <c r="AP67" s="70" t="s">
         <v>1153</v>
-      </c>
-      <c r="AP67" s="70" t="s">
-        <v>1154</v>
       </c>
       <c r="AQ67" s="70"/>
       <c r="AS67" s="7" t="s">
+        <v>1154</v>
+      </c>
+      <c r="AT67" s="18" t="s">
         <v>1155</v>
-      </c>
-      <c r="AT67" s="18" t="s">
-        <v>1156</v>
       </c>
     </row>
     <row r="68" spans="1:47" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -13414,22 +13417,22 @@
         <v>1076</v>
       </c>
       <c r="B68" s="18" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="C68" s="62"/>
       <c r="D68" s="62"/>
       <c r="E68" s="62"/>
       <c r="H68" s="7" t="s">
+        <v>1157</v>
+      </c>
+      <c r="I68" s="4" t="s">
         <v>1158</v>
       </c>
-      <c r="I68" s="4" t="s">
-        <v>1159</v>
-      </c>
       <c r="K68" s="7" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="L68" s="81" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="N68" s="3" t="s">
         <v>1034</v>
@@ -13438,19 +13441,19 @@
         <v>708</v>
       </c>
       <c r="S68" s="7" t="s">
+        <v>1159</v>
+      </c>
+      <c r="T68" s="5" t="s">
         <v>1160</v>
       </c>
-      <c r="T68" s="5" t="s">
+      <c r="U68" s="5" t="s">
         <v>1161</v>
       </c>
-      <c r="U68" s="5" t="s">
+      <c r="V68" s="5" t="s">
+        <v>1161</v>
+      </c>
+      <c r="X68" s="19" t="s">
         <v>1162</v>
-      </c>
-      <c r="V68" s="5" t="s">
-        <v>1162</v>
-      </c>
-      <c r="X68" s="19" t="s">
-        <v>1163</v>
       </c>
       <c r="Y68" s="77" t="s">
         <v>115</v>
@@ -13459,13 +13462,13 @@
         <v>50</v>
       </c>
       <c r="AB68" s="7" t="s">
+        <v>1163</v>
+      </c>
+      <c r="AC68" s="7" t="s">
         <v>1164</v>
       </c>
-      <c r="AC68" s="7" t="s">
+      <c r="AD68" s="7" t="s">
         <v>1165</v>
-      </c>
-      <c r="AD68" s="7" t="s">
-        <v>1166</v>
       </c>
       <c r="AL68" s="3" t="s">
         <v>1053</v>
@@ -13474,17 +13477,17 @@
         <v>1089</v>
       </c>
       <c r="AO68" s="70" t="s">
+        <v>1166</v>
+      </c>
+      <c r="AP68" s="70" t="s">
         <v>1167</v>
-      </c>
-      <c r="AP68" s="70" t="s">
-        <v>1168</v>
       </c>
       <c r="AQ68" s="70"/>
       <c r="AS68" s="7" t="s">
+        <v>1168</v>
+      </c>
+      <c r="AT68" s="18" t="s">
         <v>1169</v>
-      </c>
-      <c r="AT68" s="18" t="s">
-        <v>1170</v>
       </c>
     </row>
     <row r="69" spans="1:47" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -13492,40 +13495,40 @@
         <v>1090</v>
       </c>
       <c r="B69" s="18" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="C69" s="62"/>
       <c r="D69" s="62"/>
       <c r="E69" s="62"/>
       <c r="H69" s="7" t="s">
+        <v>1171</v>
+      </c>
+      <c r="I69" s="4" t="s">
         <v>1172</v>
       </c>
-      <c r="I69" s="4" t="s">
-        <v>1173</v>
-      </c>
       <c r="K69" s="7" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="L69" s="81" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="N69" s="56" t="s">
         <v>1043</v>
       </c>
       <c r="S69" s="7" t="s">
+        <v>1173</v>
+      </c>
+      <c r="T69" s="5" t="s">
         <v>1174</v>
       </c>
-      <c r="T69" s="5" t="s">
+      <c r="U69" s="5" t="s">
+        <v>1402</v>
+      </c>
+      <c r="V69" s="5" t="s">
         <v>1175</v>
       </c>
-      <c r="U69" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="V69" s="5" t="s">
+      <c r="X69" s="19" t="s">
         <v>1176</v>
-      </c>
-      <c r="X69" s="19" t="s">
-        <v>1177</v>
       </c>
       <c r="Y69" s="78" t="s">
         <v>115</v>
@@ -13534,7 +13537,7 @@
         <v>50</v>
       </c>
       <c r="AB69" s="7" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="AC69" s="7" t="s">
         <v>50</v>
@@ -13546,36 +13549,36 @@
         <v>1141</v>
       </c>
       <c r="AS69" s="7" t="s">
+        <v>1179</v>
+      </c>
+      <c r="AT69" s="18" t="s">
         <v>1180</v>
-      </c>
-      <c r="AT69" s="18" t="s">
-        <v>1181</v>
       </c>
     </row>
     <row r="70" spans="1:47" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H70" s="7" t="s">
+        <v>1181</v>
+      </c>
+      <c r="I70" s="4" t="s">
         <v>1182</v>
       </c>
-      <c r="I70" s="4" t="s">
+      <c r="K70" s="7" t="s">
+        <v>1378</v>
+      </c>
+      <c r="L70" s="7" t="s">
+        <v>1390</v>
+      </c>
+      <c r="N70" s="18" t="s">
         <v>1183</v>
       </c>
-      <c r="K70" s="7" t="s">
-        <v>1379</v>
-      </c>
-      <c r="L70" s="7" t="s">
-        <v>1391</v>
-      </c>
-      <c r="N70" s="18" t="s">
+      <c r="O70" s="18" t="s">
         <v>1184</v>
       </c>
-      <c r="O70" s="18" t="s">
+      <c r="S70" s="7" t="s">
         <v>1185</v>
       </c>
-      <c r="S70" s="7" t="s">
-        <v>1186</v>
-      </c>
       <c r="T70" s="5" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="U70" s="5" t="s">
         <v>115</v>
@@ -13593,16 +13596,16 @@
         <v>115</v>
       </c>
       <c r="AB70" s="7" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="AC70" s="7" t="s">
         <v>115</v>
       </c>
       <c r="AD70" s="7" t="s">
+        <v>1150</v>
+      </c>
+      <c r="AL70" s="4" t="s">
         <v>1151</v>
-      </c>
-      <c r="AL70" s="4" t="s">
-        <v>1152</v>
       </c>
       <c r="AN70" s="3" t="s">
         <v>1098</v>
@@ -13617,10 +13620,10 @@
         <v>1102</v>
       </c>
       <c r="AS70" s="7" t="s">
+        <v>1187</v>
+      </c>
+      <c r="AT70" s="18" t="s">
         <v>1188</v>
-      </c>
-      <c r="AT70" s="18" t="s">
-        <v>1189</v>
       </c>
     </row>
     <row r="71" spans="1:47" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -13628,19 +13631,19 @@
         <v>1095</v>
       </c>
       <c r="K71" s="7" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="L71" s="81" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="N71" s="18" t="s">
+        <v>1189</v>
+      </c>
+      <c r="O71" s="18" t="s">
+        <v>1184</v>
+      </c>
+      <c r="S71" s="7" t="s">
         <v>1190</v>
-      </c>
-      <c r="O71" s="18" t="s">
-        <v>1185</v>
-      </c>
-      <c r="S71" s="7" t="s">
-        <v>1191</v>
       </c>
       <c r="T71" s="5" t="s">
         <v>115</v>
@@ -13652,7 +13655,7 @@
         <v>50</v>
       </c>
       <c r="X71" s="19" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="Y71" s="77" t="s">
         <v>115</v>
@@ -13667,36 +13670,36 @@
         <v>1107</v>
       </c>
       <c r="AO71" s="70" t="s">
+        <v>1204</v>
+      </c>
+      <c r="AP71" s="70" t="s">
         <v>1205</v>
       </c>
-      <c r="AP71" s="70" t="s">
+      <c r="AQ71" s="70" t="s">
         <v>1206</v>
-      </c>
-      <c r="AQ71" s="70" t="s">
-        <v>1207</v>
       </c>
     </row>
     <row r="72" spans="1:47" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="18" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="B72" s="18">
         <v>0</v>
       </c>
       <c r="K72" s="7" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="L72" s="7" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="N72" s="18" t="s">
+        <v>1193</v>
+      </c>
+      <c r="O72" s="18" t="s">
+        <v>1184</v>
+      </c>
+      <c r="S72" s="7" t="s">
         <v>1194</v>
-      </c>
-      <c r="O72" s="18" t="s">
-        <v>1185</v>
-      </c>
-      <c r="S72" s="7" t="s">
-        <v>1195</v>
       </c>
       <c r="T72" s="5" t="s">
         <v>115</v>
@@ -13708,7 +13711,7 @@
         <v>50</v>
       </c>
       <c r="X72" s="19" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="Y72" s="77" t="s">
         <v>115</v>
@@ -13717,55 +13720,55 @@
         <v>50</v>
       </c>
       <c r="AL72" s="4" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="AN72" s="7" t="s">
         <v>1111</v>
       </c>
       <c r="AO72" s="70" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="AP72" s="70" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="AQ72" s="70" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="AS72" s="3" t="s">
+        <v>1196</v>
+      </c>
+      <c r="AT72" s="3" t="s">
         <v>1197</v>
-      </c>
-      <c r="AT72" s="3" t="s">
-        <v>1198</v>
       </c>
     </row>
     <row r="73" spans="1:47" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="18" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="B73" s="18">
         <v>1</v>
       </c>
       <c r="G73" s="71"/>
       <c r="H73" s="3" t="s">
+        <v>1199</v>
+      </c>
+      <c r="I73" s="3" t="s">
         <v>1200</v>
       </c>
-      <c r="I73" s="3" t="s">
+      <c r="K73" s="7" t="s">
+        <v>1381</v>
+      </c>
+      <c r="L73" s="81" t="s">
+        <v>1395</v>
+      </c>
+      <c r="N73" s="18" t="s">
         <v>1201</v>
       </c>
-      <c r="K73" s="7" t="s">
-        <v>1382</v>
-      </c>
-      <c r="L73" s="81" t="s">
-        <v>1396</v>
-      </c>
-      <c r="N73" s="18" t="s">
+      <c r="O73" s="18" t="s">
+        <v>1201</v>
+      </c>
+      <c r="S73" s="7" t="s">
         <v>1202</v>
-      </c>
-      <c r="O73" s="18" t="s">
-        <v>1202</v>
-      </c>
-      <c r="S73" s="7" t="s">
-        <v>1203</v>
       </c>
       <c r="T73" s="5" t="s">
         <v>115</v>
@@ -13777,7 +13780,7 @@
         <v>50</v>
       </c>
       <c r="X73" s="19" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="Y73" s="78" t="s">
         <v>115</v>
@@ -13789,13 +13792,13 @@
         <v>1114</v>
       </c>
       <c r="AO73" s="70" t="s">
+        <v>1215</v>
+      </c>
+      <c r="AP73" s="70" t="s">
         <v>1216</v>
       </c>
-      <c r="AP73" s="70" t="s">
-        <v>1217</v>
-      </c>
       <c r="AQ73" s="70" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="AS73" s="18" t="s">
         <v>50</v>
@@ -13804,12 +13807,12 @@
         <v>50</v>
       </c>
       <c r="AU73" s="7" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="74" spans="1:47" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="18" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="B74" s="18">
         <v>2</v>
@@ -13824,19 +13827,19 @@
         <v>115</v>
       </c>
       <c r="K74" s="7" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="L74" s="7" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="N74" s="18" t="s">
+        <v>1209</v>
+      </c>
+      <c r="O74" s="18" t="s">
+        <v>1209</v>
+      </c>
+      <c r="S74" s="7" t="s">
         <v>1210</v>
-      </c>
-      <c r="O74" s="18" t="s">
-        <v>1210</v>
-      </c>
-      <c r="S74" s="7" t="s">
-        <v>1211</v>
       </c>
       <c r="T74" s="5" t="s">
         <v>115</v>
@@ -13848,7 +13851,7 @@
         <v>115</v>
       </c>
       <c r="X74" s="19" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="Y74" s="78" t="s">
         <v>115</v>
@@ -13860,13 +13863,13 @@
         <v>1118</v>
       </c>
       <c r="AO74" s="70" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="AP74" s="70" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="AQ74" s="70" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="AS74" s="18" t="s">
         <v>115</v>
@@ -13875,7 +13878,7 @@
         <v>50</v>
       </c>
       <c r="AU74" s="7" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="75" spans="1:47" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -13889,19 +13892,19 @@
         <v>50</v>
       </c>
       <c r="K75" s="7" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="L75" s="7" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="N75" s="56" t="s">
         <v>1092</v>
       </c>
       <c r="S75" s="7" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="T75" s="5" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="U75" s="5" t="s">
         <v>115</v>
@@ -13919,16 +13922,16 @@
         <v>1122</v>
       </c>
       <c r="AO75" s="70" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="AP75" s="70" t="s">
+        <v>1216</v>
+      </c>
+      <c r="AQ75" s="70" t="s">
+        <v>1205</v>
+      </c>
+      <c r="AS75" s="18" t="s">
         <v>1217</v>
-      </c>
-      <c r="AQ75" s="70" t="s">
-        <v>1206</v>
-      </c>
-      <c r="AS75" s="18" t="s">
-        <v>1218</v>
       </c>
       <c r="AT75" s="18" t="s">
         <v>455</v>
@@ -13954,19 +13957,19 @@
         <v>115</v>
       </c>
       <c r="K76" s="7" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="L76" s="81" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="N76" s="18" t="s">
+        <v>1218</v>
+      </c>
+      <c r="O76" s="18" t="s">
+        <v>1218</v>
+      </c>
+      <c r="S76" s="7" t="s">
         <v>1219</v>
-      </c>
-      <c r="O76" s="18" t="s">
-        <v>1219</v>
-      </c>
-      <c r="S76" s="7" t="s">
-        <v>1220</v>
       </c>
       <c r="T76" s="5" t="s">
         <v>115</v>
@@ -13984,7 +13987,7 @@
         <v>115</v>
       </c>
       <c r="AU76" s="7" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="77" spans="1:47" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -13992,34 +13995,34 @@
         <v>1119</v>
       </c>
       <c r="C77" s="18" t="s">
+        <v>1222</v>
+      </c>
+      <c r="D77" s="18" t="s">
         <v>1223</v>
-      </c>
-      <c r="D77" s="18" t="s">
-        <v>1224</v>
       </c>
       <c r="G77" s="7" t="s">
         <v>1096</v>
       </c>
       <c r="H77" s="4" t="s">
+        <v>1224</v>
+      </c>
+      <c r="I77" s="4" t="s">
         <v>1225</v>
       </c>
-      <c r="I77" s="4" t="s">
+      <c r="K77" s="7" t="s">
+        <v>1385</v>
+      </c>
+      <c r="L77" s="81" t="s">
+        <v>1397</v>
+      </c>
+      <c r="N77" s="18" t="s">
         <v>1226</v>
       </c>
-      <c r="K77" s="7" t="s">
-        <v>1386</v>
-      </c>
-      <c r="L77" s="81" t="s">
-        <v>1398</v>
-      </c>
-      <c r="N77" s="18" t="s">
+      <c r="O77" s="18" t="s">
+        <v>1226</v>
+      </c>
+      <c r="S77" s="7" t="s">
         <v>1227</v>
-      </c>
-      <c r="O77" s="18" t="s">
-        <v>1227</v>
-      </c>
-      <c r="S77" s="7" t="s">
-        <v>1228</v>
       </c>
       <c r="T77" s="5" t="s">
         <v>115</v>
@@ -14037,7 +14040,7 @@
         <v>50</v>
       </c>
       <c r="AU77" s="7" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="78" spans="1:47" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -14045,10 +14048,10 @@
         <v>1138</v>
       </c>
       <c r="C78" s="18" t="s">
+        <v>1230</v>
+      </c>
+      <c r="D78" s="18" t="s">
         <v>1231</v>
-      </c>
-      <c r="D78" s="18" t="s">
-        <v>1232</v>
       </c>
       <c r="G78" s="7" t="s">
         <v>1097</v>
@@ -14057,22 +14060,22 @@
         <v>50</v>
       </c>
       <c r="I78" s="4" t="s">
+        <v>1232</v>
+      </c>
+      <c r="K78" s="7" t="s">
+        <v>1386</v>
+      </c>
+      <c r="L78" s="81" t="s">
+        <v>1398</v>
+      </c>
+      <c r="N78" s="18" t="s">
+        <v>1189</v>
+      </c>
+      <c r="O78" s="18" t="s">
         <v>1233</v>
       </c>
-      <c r="K78" s="7" t="s">
-        <v>1387</v>
-      </c>
-      <c r="L78" s="81" t="s">
-        <v>1399</v>
-      </c>
-      <c r="N78" s="18" t="s">
-        <v>1190</v>
-      </c>
-      <c r="O78" s="18" t="s">
+      <c r="S78" s="7" t="s">
         <v>1234</v>
-      </c>
-      <c r="S78" s="7" t="s">
-        <v>1235</v>
       </c>
       <c r="T78" s="5" t="s">
         <v>115</v>
@@ -14090,7 +14093,7 @@
         <v>50</v>
       </c>
       <c r="AU78" s="7" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="79" spans="1:47" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -14107,22 +14110,22 @@
         <v>1104</v>
       </c>
       <c r="H79" s="4" t="s">
+        <v>1236</v>
+      </c>
+      <c r="I79" s="4" t="s">
         <v>1237</v>
       </c>
-      <c r="I79" s="4" t="s">
+      <c r="K79" s="7" t="s">
+        <v>1387</v>
+      </c>
+      <c r="L79" s="81" t="s">
+        <v>1399</v>
+      </c>
+      <c r="O79" s="18" t="s">
         <v>1238</v>
       </c>
-      <c r="K79" s="7" t="s">
-        <v>1388</v>
-      </c>
-      <c r="L79" s="81" t="s">
-        <v>1400</v>
-      </c>
-      <c r="O79" s="18" t="s">
+      <c r="S79" s="7" t="s">
         <v>1239</v>
-      </c>
-      <c r="S79" s="7" t="s">
-        <v>1240</v>
       </c>
       <c r="T79" s="5"/>
       <c r="U79" s="5" t="s">
@@ -14135,27 +14138,27 @@
         <v>115</v>
       </c>
       <c r="AT79" s="18" t="s">
+        <v>1240</v>
+      </c>
+      <c r="AU79" s="7" t="s">
         <v>1241</v>
-      </c>
-      <c r="AU79" s="7" t="s">
-        <v>1242</v>
       </c>
     </row>
     <row r="80" spans="1:47" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B80" s="7" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="C80" s="18" t="s">
         <v>50</v>
       </c>
       <c r="D80" s="18" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="K80" s="7" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="L80" s="81" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="N80" s="56" t="s">
         <v>1110</v>
@@ -14166,7 +14169,7 @@
         <v>1139</v>
       </c>
       <c r="C81" s="18" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="D81" s="18" t="s">
         <v>115</v>
@@ -14181,13 +14184,13 @@
         <v>2</v>
       </c>
       <c r="O81" s="48" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="P81" s="56" t="s">
         <v>1113</v>
       </c>
       <c r="S81" s="3" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="V81" s="3" t="s">
         <v>681</v>
@@ -14195,19 +14198,19 @@
     </row>
     <row r="82" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B82" s="7" t="s">
+        <v>1247</v>
+      </c>
+      <c r="C82" s="18" t="s">
         <v>1248</v>
       </c>
-      <c r="C82" s="18" t="s">
+      <c r="D82" s="18" t="s">
         <v>1249</v>
-      </c>
-      <c r="D82" s="18" t="s">
-        <v>1250</v>
       </c>
       <c r="F82" s="7" t="s">
         <v>963</v>
       </c>
       <c r="G82" s="4" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="H82" s="5"/>
       <c r="I82" s="5"/>
@@ -14218,36 +14221,36 @@
         <v>15</v>
       </c>
       <c r="O82" s="48" t="s">
+        <v>1251</v>
+      </c>
+      <c r="R82" s="15" t="s">
         <v>1252</v>
       </c>
-      <c r="R82" s="15" t="s">
+      <c r="S82" s="7" t="s">
         <v>1253</v>
       </c>
-      <c r="S82" s="7" t="s">
+      <c r="T82" s="5" t="s">
         <v>1254</v>
       </c>
-      <c r="T82" s="5" t="s">
-        <v>1255</v>
-      </c>
       <c r="V82" s="7" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="83" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B83" s="7" t="s">
+        <v>1255</v>
+      </c>
+      <c r="C83" s="18" t="s">
         <v>1256</v>
       </c>
-      <c r="C83" s="18" t="s">
+      <c r="D83" s="18" t="s">
         <v>1257</v>
-      </c>
-      <c r="D83" s="18" t="s">
-        <v>1258</v>
       </c>
       <c r="F83" s="7" t="s">
         <v>983</v>
       </c>
       <c r="G83" s="5" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="H83" s="5"/>
       <c r="I83" s="5"/>
@@ -14260,19 +14263,19 @@
       <c r="O83" s="48"/>
       <c r="R83" s="10"/>
       <c r="S83" s="7" t="s">
+        <v>1259</v>
+      </c>
+      <c r="T83" s="5" t="s">
         <v>1260</v>
       </c>
-      <c r="T83" s="5" t="s">
+      <c r="V83" s="7" t="s">
         <v>1261</v>
-      </c>
-      <c r="V83" s="7" t="s">
-        <v>1262</v>
       </c>
       <c r="W83" s="3" t="s">
         <v>613</v>
       </c>
       <c r="X83" s="3" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="84" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -14280,7 +14283,7 @@
         <v>1002</v>
       </c>
       <c r="G84" s="5" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="H84" s="5"/>
       <c r="I84" s="5"/>
@@ -14293,30 +14296,30 @@
       <c r="O84" s="48"/>
       <c r="R84" s="10"/>
       <c r="S84" s="7" t="s">
+        <v>1264</v>
+      </c>
+      <c r="T84" s="5" t="s">
         <v>1265</v>
       </c>
-      <c r="T84" s="5" t="s">
+      <c r="V84" s="7" t="s">
         <v>1266</v>
       </c>
-      <c r="V84" s="7" t="s">
+      <c r="W84" s="5" t="s">
         <v>1267</v>
       </c>
-      <c r="W84" s="5" t="s">
+      <c r="X84" s="5" t="s">
         <v>1268</v>
-      </c>
-      <c r="X84" s="5" t="s">
-        <v>1269</v>
       </c>
     </row>
     <row r="85" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="F85" s="7" t="s">
         <v>1012</v>
       </c>
       <c r="G85" s="5" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="H85" s="5"/>
       <c r="I85" s="5"/>
@@ -14327,135 +14330,135 @@
         <v>1117</v>
       </c>
       <c r="O85" s="48" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="R85" s="10"/>
       <c r="S85" s="7" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="T85" s="5" t="s">
         <v>1119</v>
       </c>
       <c r="V85" s="7" t="s">
+        <v>1273</v>
+      </c>
+      <c r="W85" s="5" t="s">
         <v>1274</v>
       </c>
-      <c r="W85" s="5" t="s">
+      <c r="X85" s="5" t="s">
         <v>1275</v>
-      </c>
-      <c r="X85" s="5" t="s">
-        <v>1276</v>
       </c>
     </row>
     <row r="86" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="7" t="s">
+        <v>1276</v>
+      </c>
+      <c r="B86" s="4" t="s">
         <v>1277</v>
-      </c>
-      <c r="B86" s="4" t="s">
-        <v>1278</v>
       </c>
       <c r="M86" s="7" t="s">
         <v>1137</v>
       </c>
       <c r="N86" s="48" t="s">
+        <v>1278</v>
+      </c>
+      <c r="O86" s="48" t="s">
         <v>1279</v>
-      </c>
-      <c r="O86" s="48" t="s">
-        <v>1280</v>
       </c>
       <c r="R86" s="10"/>
       <c r="S86" s="7" t="s">
+        <v>1280</v>
+      </c>
+      <c r="T86" s="5" t="s">
         <v>1281</v>
       </c>
-      <c r="T86" s="5" t="s">
+      <c r="W86" s="5" t="s">
         <v>1282</v>
       </c>
-      <c r="W86" s="5" t="s">
+      <c r="X86" s="5" t="s">
         <v>1283</v>
-      </c>
-      <c r="X86" s="5" t="s">
-        <v>1284</v>
       </c>
     </row>
     <row r="87" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="7" t="s">
+        <v>1284</v>
+      </c>
+      <c r="B87" s="5" t="s">
         <v>1285</v>
       </c>
-      <c r="B87" s="5" t="s">
+      <c r="F87" s="3" t="s">
         <v>1286</v>
       </c>
-      <c r="F87" s="3" t="s">
+      <c r="G87" s="5" t="s">
         <v>1287</v>
-      </c>
-      <c r="G87" s="5" t="s">
-        <v>1288</v>
       </c>
       <c r="H87" s="5"/>
       <c r="R87" s="10"/>
       <c r="S87" s="7" t="s">
+        <v>1288</v>
+      </c>
+      <c r="T87" s="5" t="s">
         <v>1289</v>
       </c>
-      <c r="T87" s="5" t="s">
+      <c r="W87" s="5" t="s">
         <v>1290</v>
       </c>
-      <c r="W87" s="5" t="s">
+      <c r="X87" s="5" t="s">
         <v>1291</v>
-      </c>
-      <c r="X87" s="5" t="s">
-        <v>1292</v>
       </c>
     </row>
     <row r="88" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
+        <v>1292</v>
+      </c>
+      <c r="B88" s="5" t="s">
         <v>1293</v>
       </c>
-      <c r="B88" s="5" t="s">
+      <c r="F88" s="3" t="s">
         <v>1294</v>
       </c>
-      <c r="F88" s="3" t="s">
+      <c r="G88" s="5" t="s">
         <v>1295</v>
-      </c>
-      <c r="G88" s="5" t="s">
-        <v>1296</v>
       </c>
       <c r="H88" s="5"/>
       <c r="R88" s="15" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="S88" s="7" t="s">
+        <v>1296</v>
+      </c>
+      <c r="T88" s="4" t="s">
         <v>1297</v>
-      </c>
-      <c r="T88" s="4" t="s">
-        <v>1298</v>
       </c>
     </row>
     <row r="89" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="7" t="s">
+        <v>1298</v>
+      </c>
+      <c r="B89" s="4" t="s">
         <v>1299</v>
-      </c>
-      <c r="B89" s="4" t="s">
-        <v>1300</v>
       </c>
       <c r="R89" s="10"/>
       <c r="S89" s="7" t="s">
+        <v>1300</v>
+      </c>
+      <c r="T89" s="5" t="s">
         <v>1301</v>
-      </c>
-      <c r="T89" s="5" t="s">
-        <v>1302</v>
       </c>
     </row>
     <row r="90" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="7" t="s">
+        <v>1302</v>
+      </c>
+      <c r="B90" s="4" t="s">
         <v>1303</v>
       </c>
-      <c r="B90" s="4" t="s">
+      <c r="F90" s="3" t="s">
         <v>1304</v>
-      </c>
-      <c r="F90" s="3" t="s">
-        <v>1305</v>
       </c>
       <c r="R90" s="10"/>
       <c r="S90" s="7" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="T90" s="5" t="s">
         <v>794</v>
@@ -14463,16 +14466,16 @@
     </row>
     <row r="91" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="7" t="s">
+        <v>1306</v>
+      </c>
+      <c r="B91" s="5" t="s">
         <v>1307</v>
       </c>
-      <c r="B91" s="5" t="s">
+      <c r="F91" s="7" t="s">
         <v>1308</v>
       </c>
-      <c r="F91" s="7" t="s">
+      <c r="G91" s="4" t="s">
         <v>1309</v>
-      </c>
-      <c r="G91" s="4" t="s">
-        <v>1310</v>
       </c>
     </row>
     <row r="92" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -14480,25 +14483,25 @@
         <v>940</v>
       </c>
       <c r="B92" s="5" t="s">
+        <v>1310</v>
+      </c>
+      <c r="F92" s="7" t="s">
         <v>1311</v>
       </c>
-      <c r="F92" s="7" t="s">
+      <c r="G92" s="5" t="s">
         <v>1312</v>
       </c>
-      <c r="G92" s="5" t="s">
-        <v>1313</v>
-      </c>
       <c r="S92" s="7" t="s">
+        <v>1362</v>
+      </c>
+      <c r="T92" t="s">
         <v>1363</v>
       </c>
-      <c r="T92" t="s">
-        <v>1364</v>
-      </c>
       <c r="U92" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
       <c r="V92" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="93" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -14506,25 +14509,25 @@
         <v>960</v>
       </c>
       <c r="B93" s="5" t="s">
+        <v>1313</v>
+      </c>
+      <c r="F93" s="7" t="s">
         <v>1314</v>
       </c>
-      <c r="F93" s="7" t="s">
+      <c r="G93" s="5" t="s">
         <v>1315</v>
-      </c>
-      <c r="G93" s="5" t="s">
-        <v>1316</v>
       </c>
       <c r="S93" t="s">
         <v>443</v>
       </c>
       <c r="T93" s="5" t="s">
+        <v>1369</v>
+      </c>
+      <c r="U93" s="5" t="s">
         <v>1370</v>
       </c>
-      <c r="U93" s="5" t="s">
-        <v>1371</v>
-      </c>
       <c r="V93" s="5" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="94" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -14532,194 +14535,194 @@
         <v>952</v>
       </c>
       <c r="B94" s="4" t="s">
+        <v>1316</v>
+      </c>
+      <c r="F94" s="7" t="s">
         <v>1317</v>
       </c>
-      <c r="F94" s="7" t="s">
+      <c r="G94" s="5" t="s">
         <v>1318</v>
       </c>
-      <c r="G94" s="5" t="s">
-        <v>1319</v>
-      </c>
       <c r="S94" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="T94" s="5" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="U94" s="5" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="V94" s="5" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="95" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="7" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="S95" t="s">
+        <v>1365</v>
+      </c>
+      <c r="T95" s="5" t="s">
         <v>1366</v>
       </c>
-      <c r="T95" s="5" t="s">
-        <v>1367</v>
-      </c>
       <c r="U95" s="5" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
       <c r="V95" s="5" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="96" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="7" t="s">
+        <v>1320</v>
+      </c>
+      <c r="B96" s="5" t="s">
         <v>1321</v>
       </c>
-      <c r="B96" s="5" t="s">
+      <c r="F96" s="3" t="s">
         <v>1322</v>
-      </c>
-      <c r="F96" s="3" t="s">
-        <v>1323</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="7" t="s">
+        <v>1323</v>
+      </c>
+      <c r="B97" s="4" t="s">
         <v>1324</v>
       </c>
-      <c r="B97" s="4" t="s">
+      <c r="F97" s="7" t="s">
         <v>1325</v>
       </c>
-      <c r="F97" s="7" t="s">
+      <c r="G97" s="4" t="s">
         <v>1326</v>
-      </c>
-      <c r="G97" s="4" t="s">
-        <v>1327</v>
       </c>
     </row>
     <row r="98" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="7" t="s">
+        <v>1327</v>
+      </c>
+      <c r="B98" s="5" t="s">
         <v>1328</v>
       </c>
-      <c r="B98" s="5" t="s">
+      <c r="G98" s="5" t="s">
         <v>1329</v>
-      </c>
-      <c r="G98" s="5" t="s">
-        <v>1330</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="7" t="s">
+        <v>1330</v>
+      </c>
+      <c r="B99" s="5" t="s">
         <v>1331</v>
       </c>
-      <c r="B99" s="5" t="s">
+      <c r="G99" s="5" t="s">
         <v>1332</v>
-      </c>
-      <c r="G99" s="5" t="s">
-        <v>1333</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="7" t="s">
+        <v>1333</v>
+      </c>
+      <c r="B100" s="5" t="s">
         <v>1334</v>
       </c>
-      <c r="B100" s="5" t="s">
+      <c r="G100" s="5" t="s">
         <v>1335</v>
-      </c>
-      <c r="G100" s="5" t="s">
-        <v>1336</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F101" s="7" t="s">
+        <v>1336</v>
+      </c>
+      <c r="G101" s="4" t="s">
         <v>1337</v>
-      </c>
-      <c r="G101" s="4" t="s">
-        <v>1338</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
+        <v>1338</v>
+      </c>
+      <c r="B102" s="3" t="s">
         <v>1339</v>
       </c>
-      <c r="B102" s="3" t="s">
+      <c r="C102" s="3" t="s">
         <v>1340</v>
       </c>
-      <c r="C102" s="3" t="s">
+      <c r="G102" s="5" t="s">
         <v>1341</v>
-      </c>
-      <c r="G102" s="5" t="s">
-        <v>1342</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="7" t="s">
+        <v>1342</v>
+      </c>
+      <c r="F103" s="7" t="s">
         <v>1343</v>
       </c>
-      <c r="F103" s="7" t="s">
+      <c r="G103" s="5" t="s">
         <v>1344</v>
-      </c>
-      <c r="G103" s="5" t="s">
-        <v>1345</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="7" t="s">
+        <v>1345</v>
+      </c>
+      <c r="G104" s="4" t="s">
         <v>1346</v>
-      </c>
-      <c r="G104" s="4" t="s">
-        <v>1347</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="7" t="s">
+        <v>1347</v>
+      </c>
+      <c r="G105" s="5" t="s">
         <v>1348</v>
-      </c>
-      <c r="G105" s="5" t="s">
-        <v>1349</v>
       </c>
     </row>
     <row r="106" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="7" t="s">
+        <v>1349</v>
+      </c>
+      <c r="G106" s="5" t="s">
         <v>1350</v>
-      </c>
-      <c r="G106" s="5" t="s">
-        <v>1351</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="7" t="s">
+        <v>1351</v>
+      </c>
+      <c r="C107" s="7" t="s">
         <v>1352</v>
       </c>
-      <c r="C107" s="7" t="s">
+      <c r="G107" s="5" t="s">
         <v>1353</v>
-      </c>
-      <c r="G107" s="5" t="s">
-        <v>1354</v>
       </c>
     </row>
     <row r="108" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="7" t="s">
+        <v>1354</v>
+      </c>
+      <c r="C108" s="5" t="s">
         <v>1355</v>
-      </c>
-      <c r="C108" s="5" t="s">
-        <v>1356</v>
       </c>
     </row>
     <row r="109" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C109" s="5" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="110" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C110" s="5" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="111" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C111" s="5" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="112" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updated written drill sheet
</commit_message>
<xml_diff>
--- a/written-exam-memory-drills.xlsx
+++ b/written-exam-memory-drills.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-37905" yWindow="1035" windowWidth="34755" windowHeight="11550" tabRatio="500"/>
+    <workbookView xWindow="-37908" yWindow="1032" windowWidth="34752" windowHeight="11556" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="answers" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1758" uniqueCount="1489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1760" uniqueCount="1491">
   <si>
     <t>bgp best-path</t>
   </si>
@@ -4667,6 +4667,12 @@
   </si>
   <si>
     <t>route must be listed in action list (advertise or inject) AND condition map (exist/nonexist)</t>
+  </si>
+  <si>
+    <t>ff02::16</t>
+  </si>
+  <si>
+    <t>all mldv2-capable routers</t>
   </si>
 </sst>
 </file>
@@ -5259,73 +5265,73 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BG997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD67" zoomScale="146" zoomScaleNormal="146" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="AF70" sqref="AF70"/>
+    <sheetView tabSelected="1" topLeftCell="N10" zoomScale="146" zoomScaleNormal="146" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="30.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.140625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="4.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.140625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="28.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="41.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.140625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="26.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="28.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="4.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.109375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="28.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="41.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.109375" style="4" customWidth="1"/>
+    <col min="13" max="13" width="26.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.140625" style="4" customWidth="1"/>
-    <col min="17" max="17" width="38.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="27.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="37.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.140625" style="4" customWidth="1"/>
-    <col min="21" max="21" width="25.140625" style="3" customWidth="1"/>
-    <col min="22" max="22" width="20.42578125" style="3" customWidth="1"/>
-    <col min="23" max="23" width="28.85546875" style="3" customWidth="1"/>
-    <col min="24" max="24" width="22.28515625" style="3" customWidth="1"/>
-    <col min="25" max="25" width="5.140625" style="4" customWidth="1"/>
-    <col min="26" max="26" width="29.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="51.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="30.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="49.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="5.140625" style="4" customWidth="1"/>
-    <col min="31" max="31" width="31.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="31.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="29.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="29.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="27.7109375" style="3" customWidth="1"/>
-    <col min="37" max="37" width="5.140625" style="4" customWidth="1"/>
-    <col min="38" max="38" width="24.28515625" style="3" customWidth="1"/>
-    <col min="39" max="39" width="25.42578125" style="3" customWidth="1"/>
-    <col min="40" max="40" width="18.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="26.42578125" style="3" customWidth="1"/>
-    <col min="42" max="42" width="5.140625" style="4" customWidth="1"/>
-    <col min="43" max="43" width="25.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="37.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="26.42578125" style="3" customWidth="1"/>
-    <col min="46" max="46" width="20.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="5.140625" style="4" customWidth="1"/>
-    <col min="48" max="48" width="28.140625" style="3" customWidth="1"/>
+    <col min="16" max="16" width="5.109375" style="4" customWidth="1"/>
+    <col min="17" max="17" width="38.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="27.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="37.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.109375" style="4" customWidth="1"/>
+    <col min="21" max="21" width="25.109375" style="3" customWidth="1"/>
+    <col min="22" max="22" width="20.44140625" style="3" customWidth="1"/>
+    <col min="23" max="23" width="28.88671875" style="3" customWidth="1"/>
+    <col min="24" max="24" width="22.33203125" style="3" customWidth="1"/>
+    <col min="25" max="25" width="5.109375" style="4" customWidth="1"/>
+    <col min="26" max="26" width="29.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="51.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="30.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="49.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="5.109375" style="4" customWidth="1"/>
+    <col min="31" max="31" width="31.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="31.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="29.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="29.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="27.6640625" style="3" customWidth="1"/>
+    <col min="37" max="37" width="5.109375" style="4" customWidth="1"/>
+    <col min="38" max="38" width="24.33203125" style="3" customWidth="1"/>
+    <col min="39" max="39" width="25.44140625" style="3" customWidth="1"/>
+    <col min="40" max="40" width="18.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="26.44140625" style="3" customWidth="1"/>
+    <col min="42" max="42" width="5.109375" style="4" customWidth="1"/>
+    <col min="43" max="43" width="25.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="37.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="26.44140625" style="3" customWidth="1"/>
+    <col min="46" max="46" width="20.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="5.109375" style="4" customWidth="1"/>
+    <col min="48" max="48" width="28.109375" style="3" customWidth="1"/>
     <col min="49" max="49" width="24" style="3" customWidth="1"/>
-    <col min="50" max="50" width="32.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="17.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="5.140625" style="4" customWidth="1"/>
-    <col min="53" max="53" width="28.85546875" style="3" customWidth="1"/>
-    <col min="54" max="54" width="26.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="28.42578125" style="3" customWidth="1"/>
-    <col min="56" max="58" width="14.42578125" style="3"/>
-    <col min="59" max="59" width="14.42578125" style="35"/>
-    <col min="60" max="16384" width="14.42578125" style="3"/>
+    <col min="50" max="50" width="32.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="17.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="5.109375" style="4" customWidth="1"/>
+    <col min="53" max="53" width="28.88671875" style="3" customWidth="1"/>
+    <col min="54" max="54" width="26.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="28.44140625" style="3" customWidth="1"/>
+    <col min="56" max="58" width="14.44140625" style="3"/>
+    <col min="59" max="59" width="14.44140625" style="35"/>
+    <col min="60" max="16384" width="14.44140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5393,7 +5399,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="2" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
         <v>17</v>
       </c>
@@ -5482,7 +5488,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="3" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
         <v>42</v>
       </c>
@@ -5565,7 +5571,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="4" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="8" t="s">
         <v>58</v>
       </c>
@@ -5651,7 +5657,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="5" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
         <v>76</v>
       </c>
@@ -5725,7 +5731,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="6" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
         <v>87</v>
       </c>
@@ -5805,7 +5811,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="7" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="8" t="s">
         <v>98</v>
       </c>
@@ -5900,7 +5906,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="8" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="8" t="s">
         <v>111</v>
       </c>
@@ -5961,7 +5967,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="9" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="8" t="s">
         <v>1373</v>
       </c>
@@ -6029,7 +6035,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="10" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="8" t="s">
         <v>128</v>
       </c>
@@ -6095,7 +6101,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="11" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="8" t="s">
         <v>132</v>
       </c>
@@ -6168,7 +6174,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="12" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="8" t="s">
         <v>1214</v>
       </c>
@@ -6239,7 +6245,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="13" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="8" t="s">
         <v>1215</v>
       </c>
@@ -6294,7 +6300,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="14" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H14" s="8" t="s">
         <v>169</v>
       </c>
@@ -6356,7 +6362,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="15" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="34" t="s">
         <v>147</v>
       </c>
@@ -6420,7 +6426,7 @@
       </c>
       <c r="BE15" s="7"/>
     </row>
-    <row r="16" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="27" t="s">
         <v>157</v>
       </c>
@@ -6509,7 +6515,7 @@
       </c>
       <c r="BE16" s="7"/>
     </row>
-    <row r="17" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="27" t="s">
         <v>168</v>
       </c>
@@ -6587,7 +6593,7 @@
       </c>
       <c r="BE17" s="7"/>
     </row>
-    <row r="18" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="27" t="s">
         <v>178</v>
       </c>
@@ -6651,7 +6657,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="19" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="27" t="s">
         <v>190</v>
       </c>
@@ -6721,7 +6727,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="20" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H20" s="8" t="s">
         <v>250</v>
       </c>
@@ -6790,7 +6796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H21" s="8" t="s">
         <v>260</v>
       </c>
@@ -6840,7 +6846,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="22" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="6" t="s">
         <v>235</v>
       </c>
@@ -6883,7 +6889,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="23" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="7" t="s">
         <v>248</v>
       </c>
@@ -6939,7 +6945,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="24" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="8" t="s">
         <v>164</v>
       </c>
@@ -6956,10 +6962,10 @@
         <v>660</v>
       </c>
       <c r="Q24" s="9" t="s">
-        <v>270</v>
+        <v>1489</v>
       </c>
       <c r="R24" s="7" t="s">
-        <v>276</v>
+        <v>1490</v>
       </c>
       <c r="S24" s="7"/>
       <c r="U24" s="9" t="s">
@@ -7014,7 +7020,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="25" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="7" t="s">
         <v>272</v>
       </c>
@@ -7030,6 +7036,13 @@
       <c r="M25" s="7" t="s">
         <v>675</v>
       </c>
+      <c r="Q25" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="R25" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="S25" s="7"/>
       <c r="U25" s="9" t="s">
         <v>444</v>
       </c>
@@ -7082,7 +7095,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="26" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="7" t="s">
         <v>286</v>
       </c>
@@ -7095,12 +7108,6 @@
       </c>
       <c r="M26" s="7" t="s">
         <v>679</v>
-      </c>
-      <c r="Q26" s="6" t="s">
-        <v>295</v>
-      </c>
-      <c r="R26" s="6" t="s">
-        <v>297</v>
       </c>
       <c r="U26" s="9" t="s">
         <v>460</v>
@@ -7154,7 +7161,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="27" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="7" t="s">
         <v>293</v>
       </c>
@@ -7170,11 +7177,11 @@
       <c r="M27" s="7" t="s">
         <v>688</v>
       </c>
-      <c r="Q27" s="7" t="s">
-        <v>308</v>
-      </c>
-      <c r="R27" s="7" t="s">
-        <v>309</v>
+      <c r="Q27" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="R27" s="6" t="s">
+        <v>297</v>
       </c>
       <c r="U27" s="9" t="s">
         <v>475</v>
@@ -7231,7 +7238,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="28" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H28" s="7" t="s">
         <v>1179</v>
       </c>
@@ -7242,10 +7249,10 @@
         <v>697</v>
       </c>
       <c r="Q28" s="7" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="R28" s="7" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="U28" s="9" t="s">
         <v>489</v>
@@ -7304,7 +7311,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="29" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="6" t="s">
         <v>315</v>
       </c>
@@ -7318,10 +7325,10 @@
         <v>713</v>
       </c>
       <c r="Q29" s="7" t="s">
-        <v>329</v>
+        <v>317</v>
       </c>
       <c r="R29" s="7" t="s">
-        <v>330</v>
+        <v>318</v>
       </c>
       <c r="U29" s="9" t="s">
         <v>502</v>
@@ -7361,7 +7368,7 @@
         <v>1439</v>
       </c>
     </row>
-    <row r="30" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="7" t="s">
         <v>326</v>
       </c>
@@ -7374,9 +7381,11 @@
       <c r="J30" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="Q30" s="7"/>
+      <c r="Q30" s="7" t="s">
+        <v>329</v>
+      </c>
       <c r="R30" s="7" t="s">
-        <v>344</v>
+        <v>330</v>
       </c>
       <c r="AL30" s="6" t="s">
         <v>447</v>
@@ -7397,7 +7406,7 @@
         <v>1156</v>
       </c>
     </row>
-    <row r="31" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="7" t="s">
         <v>339</v>
       </c>
@@ -7415,6 +7424,10 @@
       </c>
       <c r="N31" s="6" t="s">
         <v>712</v>
+      </c>
+      <c r="Q31" s="7"/>
+      <c r="R31" s="7" t="s">
+        <v>344</v>
       </c>
       <c r="U31" s="1" t="s">
         <v>515</v>
@@ -7460,7 +7473,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="32" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="7" t="s">
         <v>353</v>
       </c>
@@ -7479,12 +7492,6 @@
       <c r="N32" s="7" t="s">
         <v>740</v>
       </c>
-      <c r="Q32" s="6" t="s">
-        <v>359</v>
-      </c>
-      <c r="S32" s="9" t="s">
-        <v>1022</v>
-      </c>
       <c r="U32" s="3" t="s">
         <v>532</v>
       </c>
@@ -7525,7 +7532,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="33" spans="2:53" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:53" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="7" t="s">
         <v>362</v>
       </c>
@@ -7544,14 +7551,11 @@
       <c r="N33" s="7" t="s">
         <v>746</v>
       </c>
-      <c r="Q33" s="9" t="s">
-        <v>376</v>
-      </c>
-      <c r="R33" s="9" t="s">
-        <v>377</v>
+      <c r="Q33" s="6" t="s">
+        <v>359</v>
       </c>
       <c r="S33" s="9" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="U33" s="8" t="s">
         <v>562</v>
@@ -7592,7 +7596,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="34" spans="2:53" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:53" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="7" t="s">
         <v>378</v>
       </c>
@@ -7609,11 +7613,14 @@
       <c r="N34" s="7" t="s">
         <v>753</v>
       </c>
-      <c r="Q34" s="8" t="s">
-        <v>396</v>
-      </c>
-      <c r="R34" s="8" t="s">
-        <v>396</v>
+      <c r="Q34" s="9" t="s">
+        <v>376</v>
+      </c>
+      <c r="R34" s="9" t="s">
+        <v>377</v>
+      </c>
+      <c r="S34" s="9" t="s">
+        <v>1023</v>
       </c>
       <c r="U34" s="8" t="s">
         <v>577</v>
@@ -7657,7 +7664,7 @@
         <v>1147</v>
       </c>
     </row>
-    <row r="35" spans="2:53" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:53" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="24" t="s">
         <v>386</v>
       </c>
@@ -7674,10 +7681,10 @@
         <v>773</v>
       </c>
       <c r="Q35" s="8" t="s">
-        <v>406</v>
+        <v>396</v>
       </c>
       <c r="R35" s="8" t="s">
-        <v>406</v>
+        <v>396</v>
       </c>
       <c r="Z35" s="28" t="s">
         <v>399</v>
@@ -7723,7 +7730,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="36" spans="2:53" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:53" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="6" t="s">
         <v>400</v>
       </c>
@@ -7737,10 +7744,10 @@
         <v>794</v>
       </c>
       <c r="Q36" s="8" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
       <c r="R36" s="8" t="s">
-        <v>416</v>
+        <v>406</v>
       </c>
       <c r="U36" s="3" t="s">
         <v>593</v>
@@ -7779,7 +7786,7 @@
         <v>1157</v>
       </c>
     </row>
-    <row r="37" spans="2:53" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:53" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="7" t="s">
         <v>411</v>
       </c>
@@ -7796,10 +7803,10 @@
         <v>646</v>
       </c>
       <c r="Q37" s="8" t="s">
-        <v>427</v>
+        <v>415</v>
       </c>
       <c r="R37" s="8" t="s">
-        <v>428</v>
+        <v>416</v>
       </c>
       <c r="U37" s="8" t="s">
         <v>562</v>
@@ -7840,7 +7847,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="38" spans="2:53" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:53" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="7" t="s">
         <v>424</v>
       </c>
@@ -7859,11 +7866,11 @@
       <c r="N38" s="7" t="s">
         <v>812</v>
       </c>
-      <c r="Q38" s="24" t="s">
-        <v>440</v>
-      </c>
-      <c r="R38" s="24" t="s">
-        <v>441</v>
+      <c r="Q38" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="R38" s="8" t="s">
+        <v>428</v>
       </c>
       <c r="U38" s="8" t="s">
         <v>615</v>
@@ -7901,7 +7908,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="39" spans="2:53" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:53" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="7" t="s">
         <v>443</v>
       </c>
@@ -7919,6 +7926,12 @@
       </c>
       <c r="N39" s="7" t="s">
         <v>823</v>
+      </c>
+      <c r="Q39" s="24" t="s">
+        <v>440</v>
+      </c>
+      <c r="R39" s="24" t="s">
+        <v>441</v>
       </c>
       <c r="Z39" s="28" t="s">
         <v>450</v>
@@ -7967,7 +7980,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="40" spans="2:53" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:53" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="7" t="s">
         <v>458</v>
       </c>
@@ -7983,9 +7996,6 @@
       </c>
       <c r="N40" s="7" t="s">
         <v>833</v>
-      </c>
-      <c r="Q40" s="6" t="s">
-        <v>473</v>
       </c>
       <c r="V40" s="6" t="s">
         <v>517</v>
@@ -8037,7 +8047,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="41" spans="2:53" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:53" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="7" t="s">
         <v>472</v>
       </c>
@@ -8051,11 +8061,8 @@
         <v>77</v>
       </c>
       <c r="O41" s="9"/>
-      <c r="Q41" s="8" t="s">
-        <v>488</v>
-      </c>
-      <c r="R41" s="8" t="s">
-        <v>490</v>
+      <c r="Q41" s="6" t="s">
+        <v>473</v>
       </c>
       <c r="U41" s="16" t="s">
         <v>283</v>
@@ -8112,7 +8119,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="42" spans="2:53" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:53" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H42" s="12" t="s">
         <v>520</v>
       </c>
@@ -8123,10 +8130,10 @@
         <v>849</v>
       </c>
       <c r="Q42" s="8" t="s">
-        <v>508</v>
+        <v>488</v>
       </c>
       <c r="R42" s="8" t="s">
-        <v>509</v>
+        <v>490</v>
       </c>
       <c r="U42" s="16" t="s">
         <v>563</v>
@@ -8187,7 +8194,7 @@
         <v>1152</v>
       </c>
     </row>
-    <row r="43" spans="2:53" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:53" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="6" t="s">
         <v>496</v>
       </c>
@@ -8207,10 +8214,10 @@
         <v>75</v>
       </c>
       <c r="Q43" s="8" t="s">
-        <v>523</v>
+        <v>508</v>
       </c>
       <c r="R43" s="8" t="s">
-        <v>524</v>
+        <v>509</v>
       </c>
       <c r="U43" s="16" t="s">
         <v>572</v>
@@ -8252,7 +8259,7 @@
         <v>1153</v>
       </c>
     </row>
-    <row r="44" spans="2:53" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:53" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="7" t="s">
         <v>519</v>
       </c>
@@ -8274,6 +8281,12 @@
       <c r="O44" s="7" t="s">
         <v>35</v>
       </c>
+      <c r="Q44" s="8" t="s">
+        <v>523</v>
+      </c>
+      <c r="R44" s="8" t="s">
+        <v>524</v>
+      </c>
       <c r="U44" s="16" t="s">
         <v>582</v>
       </c>
@@ -8296,7 +8309,7 @@
         <v>1154</v>
       </c>
     </row>
-    <row r="45" spans="2:53" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:53" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="7" t="s">
         <v>537</v>
       </c>
@@ -8317,9 +8330,6 @@
       </c>
       <c r="O45" s="7" t="s">
         <v>75</v>
-      </c>
-      <c r="Q45" s="6" t="s">
-        <v>530</v>
       </c>
       <c r="Z45" s="28" t="s">
         <v>518</v>
@@ -8359,7 +8369,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="46" spans="2:53" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:53" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="7" t="s">
         <v>548</v>
       </c>
@@ -8381,8 +8391,8 @@
       <c r="O46" s="7" t="s">
         <v>870</v>
       </c>
-      <c r="Q46" s="8" t="s">
-        <v>558</v>
+      <c r="Q46" s="6" t="s">
+        <v>530</v>
       </c>
       <c r="U46" s="6" t="s">
         <v>795</v>
@@ -8431,7 +8441,7 @@
       </c>
       <c r="AX46" s="7"/>
     </row>
-    <row r="47" spans="2:53" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:53" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="7" t="s">
         <v>556</v>
       </c>
@@ -8452,7 +8462,7 @@
         <v>876</v>
       </c>
       <c r="Q47" s="8" t="s">
-        <v>570</v>
+        <v>558</v>
       </c>
       <c r="U47" s="9" t="s">
         <v>1016</v>
@@ -8506,7 +8516,7 @@
         <v>1164</v>
       </c>
     </row>
-    <row r="48" spans="2:53" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:53" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="7" t="s">
         <v>568</v>
       </c>
@@ -8523,8 +8533,8 @@
       <c r="O48" s="7" t="s">
         <v>880</v>
       </c>
-      <c r="Q48" s="7" t="s">
-        <v>580</v>
+      <c r="Q48" s="8" t="s">
+        <v>570</v>
       </c>
       <c r="U48" s="9" t="s">
         <v>813</v>
@@ -8572,7 +8582,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="49" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H49" s="7" t="s">
         <v>685</v>
       </c>
@@ -8583,8 +8593,8 @@
         <v>612</v>
       </c>
       <c r="O49" s="9"/>
-      <c r="Q49" s="8" t="s">
-        <v>597</v>
+      <c r="Q49" s="7" t="s">
+        <v>580</v>
       </c>
       <c r="U49" s="9" t="s">
         <v>824</v>
@@ -8638,7 +8648,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="50" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="6" t="s">
         <v>590</v>
       </c>
@@ -8661,6 +8671,9 @@
       <c r="M50" s="6" t="s">
         <v>604</v>
       </c>
+      <c r="Q50" s="8" t="s">
+        <v>597</v>
+      </c>
       <c r="U50" s="9" t="s">
         <v>836</v>
       </c>
@@ -8704,7 +8717,7 @@
         <v>1160</v>
       </c>
     </row>
-    <row r="51" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B51" s="8" t="s">
         <v>601</v>
       </c>
@@ -8729,12 +8742,6 @@
       </c>
       <c r="N51" s="3" t="s">
         <v>617</v>
-      </c>
-      <c r="R51" s="6" t="s">
-        <v>721</v>
-      </c>
-      <c r="S51" s="6" t="s">
-        <v>480</v>
       </c>
       <c r="U51" s="9" t="s">
         <v>841</v>
@@ -8779,7 +8786,7 @@
       </c>
       <c r="AX51" s="7"/>
     </row>
-    <row r="52" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="8" t="s">
         <v>609</v>
       </c>
@@ -8805,8 +8812,11 @@
       <c r="N52" s="8" t="s">
         <v>637</v>
       </c>
-      <c r="R52" s="24" t="s">
-        <v>728</v>
+      <c r="R52" s="6" t="s">
+        <v>721</v>
+      </c>
+      <c r="S52" s="6" t="s">
+        <v>480</v>
       </c>
       <c r="U52" s="9" t="s">
         <v>845</v>
@@ -8850,7 +8860,7 @@
         <v>1165</v>
       </c>
     </row>
-    <row r="53" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="7" t="s">
         <v>623</v>
       </c>
@@ -8868,11 +8878,8 @@
       <c r="N53" s="8" t="s">
         <v>650</v>
       </c>
-      <c r="R53" s="8" t="s">
-        <v>834</v>
-      </c>
-      <c r="S53" s="8" t="s">
-        <v>835</v>
+      <c r="R53" s="24" t="s">
+        <v>728</v>
       </c>
       <c r="U53" s="9" t="s">
         <v>851</v>
@@ -8928,7 +8935,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="54" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G54" s="3"/>
       <c r="H54" s="6" t="s">
         <v>323</v>
@@ -8942,10 +8949,10 @@
       <c r="N54" s="8" t="s">
         <v>662</v>
       </c>
-      <c r="R54" s="7" t="s">
-        <v>840</v>
-      </c>
-      <c r="S54" s="7" t="s">
+      <c r="R54" s="8" t="s">
+        <v>834</v>
+      </c>
+      <c r="S54" s="8" t="s">
         <v>835</v>
       </c>
       <c r="U54" s="9" t="s">
@@ -8991,7 +8998,7 @@
         <v>1162</v>
       </c>
     </row>
-    <row r="55" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B55" s="6" t="s">
         <v>1182</v>
       </c>
@@ -9003,7 +9010,7 @@
         <v>702</v>
       </c>
       <c r="R55" s="7" t="s">
-        <v>844</v>
+        <v>840</v>
       </c>
       <c r="S55" s="7" t="s">
         <v>835</v>
@@ -9046,7 +9053,7 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="56" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B56" s="6" t="s">
         <v>1183</v>
       </c>
@@ -9068,10 +9075,10 @@
       </c>
       <c r="N56" s="9"/>
       <c r="R56" s="7" t="s">
-        <v>850</v>
+        <v>844</v>
       </c>
       <c r="S56" s="7" t="s">
-        <v>850</v>
+        <v>835</v>
       </c>
       <c r="U56" s="9" t="s">
         <v>865</v>
@@ -9113,7 +9120,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="57" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B57" s="8" t="s">
         <v>673</v>
       </c>
@@ -9138,11 +9145,11 @@
       <c r="N57" s="8" t="s">
         <v>1011</v>
       </c>
-      <c r="R57" s="8" t="s">
-        <v>857</v>
-      </c>
-      <c r="S57" s="8" t="s">
-        <v>857</v>
+      <c r="R57" s="7" t="s">
+        <v>850</v>
+      </c>
+      <c r="S57" s="7" t="s">
+        <v>850</v>
       </c>
       <c r="U57" s="9" t="s">
         <v>872</v>
@@ -9199,7 +9206,7 @@
         <v>1335</v>
       </c>
     </row>
-    <row r="58" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B58" s="8" t="s">
         <v>673</v>
       </c>
@@ -9224,8 +9231,11 @@
       <c r="N58" s="8" t="s">
         <v>1010</v>
       </c>
-      <c r="R58" s="24" t="s">
-        <v>758</v>
+      <c r="R58" s="8" t="s">
+        <v>857</v>
+      </c>
+      <c r="S58" s="8" t="s">
+        <v>857</v>
       </c>
       <c r="U58" s="9" t="s">
         <v>878</v>
@@ -9277,7 +9287,7 @@
       </c>
       <c r="BE58" s="26"/>
     </row>
-    <row r="59" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B59" s="7" t="s">
         <v>674</v>
       </c>
@@ -9297,11 +9307,8 @@
       <c r="N59" s="8" t="s">
         <v>1005</v>
       </c>
-      <c r="R59" s="8" t="s">
-        <v>864</v>
-      </c>
-      <c r="S59" s="8" t="s">
-        <v>864</v>
+      <c r="R59" s="24" t="s">
+        <v>758</v>
       </c>
       <c r="U59" s="9" t="s">
         <v>882</v>
@@ -9339,7 +9346,7 @@
       </c>
       <c r="BE59" s="26"/>
     </row>
-    <row r="60" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B60" s="8" t="s">
         <v>673</v>
       </c>
@@ -9362,11 +9369,11 @@
       <c r="N60" s="8" t="s">
         <v>1009</v>
       </c>
-      <c r="R60" s="7" t="s">
-        <v>871</v>
+      <c r="R60" s="8" t="s">
+        <v>864</v>
       </c>
       <c r="S60" s="8" t="s">
-        <v>871</v>
+        <v>864</v>
       </c>
       <c r="Z60" s="7" t="s">
         <v>358</v>
@@ -9400,7 +9407,7 @@
       </c>
       <c r="BE60" s="26"/>
     </row>
-    <row r="61" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B61" s="8" t="s">
         <v>708</v>
       </c>
@@ -9427,10 +9434,10 @@
         <v>1006</v>
       </c>
       <c r="R61" s="7" t="s">
-        <v>840</v>
-      </c>
-      <c r="S61" s="7" t="s">
-        <v>877</v>
+        <v>871</v>
+      </c>
+      <c r="S61" s="8" t="s">
+        <v>871</v>
       </c>
       <c r="V61" s="6" t="s">
         <v>888</v>
@@ -9470,7 +9477,7 @@
       </c>
       <c r="BE61" s="26"/>
     </row>
-    <row r="62" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B62" s="7" t="s">
         <v>710</v>
       </c>
@@ -9496,8 +9503,11 @@
       <c r="N62" s="8" t="s">
         <v>1010</v>
       </c>
+      <c r="R62" s="7" t="s">
+        <v>840</v>
+      </c>
       <c r="S62" s="7" t="s">
-        <v>881</v>
+        <v>877</v>
       </c>
       <c r="U62" s="13" t="s">
         <v>894</v>
@@ -9537,7 +9547,7 @@
       </c>
       <c r="BE62" s="26"/>
     </row>
-    <row r="63" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B63" s="7" t="s">
         <v>674</v>
       </c>
@@ -9563,8 +9573,8 @@
       <c r="N63" s="8" t="s">
         <v>1007</v>
       </c>
-      <c r="R63" s="24" t="s">
-        <v>774</v>
+      <c r="S63" s="7" t="s">
+        <v>881</v>
       </c>
       <c r="U63" s="16"/>
       <c r="V63" s="9" t="s">
@@ -9593,7 +9603,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="64" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B64" s="8" t="s">
         <v>710</v>
       </c>
@@ -9618,14 +9628,8 @@
       <c r="N64" s="8" t="s">
         <v>1008</v>
       </c>
-      <c r="Q64" s="9" t="s">
-        <v>776</v>
-      </c>
-      <c r="R64" s="26">
-        <v>2</v>
-      </c>
-      <c r="S64" s="26" t="s">
-        <v>887</v>
+      <c r="R64" s="24" t="s">
+        <v>774</v>
       </c>
       <c r="U64" s="16"/>
       <c r="V64" s="9" t="s">
@@ -9659,7 +9663,7 @@
       </c>
       <c r="AS64" s="6"/>
     </row>
-    <row r="65" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B65" s="7" t="s">
         <v>710</v>
       </c>
@@ -9679,13 +9683,13 @@
         <v>1010</v>
       </c>
       <c r="Q65" s="9" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="R65" s="26">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="S65" s="26" t="s">
-        <v>893</v>
+        <v>887</v>
       </c>
       <c r="U65" s="16"/>
       <c r="V65" s="9" t="s">
@@ -9720,7 +9724,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="66" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="J66" s="6" t="s">
         <v>928</v>
       </c>
@@ -9734,12 +9738,14 @@
         <v>1012</v>
       </c>
       <c r="Q66" s="9" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="R66" s="26">
-        <v>20</v>
-      </c>
-      <c r="S66" s="26"/>
+        <v>15</v>
+      </c>
+      <c r="S66" s="26" t="s">
+        <v>893</v>
+      </c>
       <c r="U66" s="16"/>
       <c r="V66" s="9" t="s">
         <v>922</v>
@@ -9764,7 +9770,7 @@
       </c>
       <c r="AO66" s="7"/>
     </row>
-    <row r="67" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B67" s="13" t="s">
         <v>1331</v>
       </c>
@@ -9781,10 +9787,10 @@
         <v>1013</v>
       </c>
       <c r="Q67" s="9" t="s">
-        <v>788</v>
+        <v>783</v>
       </c>
       <c r="R67" s="26">
-        <v>300</v>
+        <v>20</v>
       </c>
       <c r="S67" s="26"/>
       <c r="U67" s="16"/>
@@ -9817,7 +9823,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="68" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B68" s="9">
         <v>0</v>
       </c>
@@ -9831,14 +9837,12 @@
         <v>1014</v>
       </c>
       <c r="Q68" s="9" t="s">
-        <v>792</v>
-      </c>
-      <c r="R68" s="26" t="s">
-        <v>780</v>
-      </c>
-      <c r="S68" s="26" t="s">
-        <v>913</v>
-      </c>
+        <v>788</v>
+      </c>
+      <c r="R68" s="26">
+        <v>300</v>
+      </c>
+      <c r="S68" s="26"/>
       <c r="U68" s="13" t="s">
         <v>903</v>
       </c>
@@ -9883,7 +9887,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="69" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B69" s="9">
         <v>1</v>
       </c>
@@ -9900,13 +9904,13 @@
         <v>1015</v>
       </c>
       <c r="Q69" s="9" t="s">
-        <v>797</v>
+        <v>792</v>
       </c>
       <c r="R69" s="26" t="s">
-        <v>920</v>
+        <v>780</v>
       </c>
       <c r="S69" s="26" t="s">
-        <v>921</v>
+        <v>913</v>
       </c>
       <c r="U69" s="16"/>
       <c r="V69" s="9" t="s">
@@ -9943,7 +9947,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="70" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B70" s="9">
         <v>2</v>
       </c>
@@ -9957,6 +9961,15 @@
         <v>958</v>
       </c>
       <c r="M70" s="3"/>
+      <c r="Q70" s="9" t="s">
+        <v>797</v>
+      </c>
+      <c r="R70" s="26" t="s">
+        <v>920</v>
+      </c>
+      <c r="S70" s="26" t="s">
+        <v>921</v>
+      </c>
       <c r="U70" s="16"/>
       <c r="V70" s="9" t="s">
         <v>945</v>
@@ -9993,7 +10006,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="71" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="J71" s="3"/>
       <c r="K71" s="8" t="s">
         <v>961</v>
@@ -10002,12 +10015,6 @@
         <v>566</v>
       </c>
       <c r="O71" s="31"/>
-      <c r="R71" s="29" t="s">
-        <v>756</v>
-      </c>
-      <c r="S71" s="29" t="s">
-        <v>760</v>
-      </c>
       <c r="AA71" s="3"/>
       <c r="AE71" s="3" t="s">
         <v>1460</v>
@@ -10034,7 +10041,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="72" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C72" s="6" t="s">
         <v>778</v>
       </c>
@@ -10052,14 +10059,11 @@
         <v>599</v>
       </c>
       <c r="O72" s="31"/>
-      <c r="Q72" s="16" t="s">
-        <v>805</v>
-      </c>
-      <c r="R72" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="S72" s="30" t="s">
-        <v>35</v>
+      <c r="R72" s="29" t="s">
+        <v>756</v>
+      </c>
+      <c r="S72" s="29" t="s">
+        <v>760</v>
       </c>
       <c r="U72" s="6" t="s">
         <v>487</v>
@@ -10098,7 +10102,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="73" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B73" s="16" t="s">
         <v>782</v>
       </c>
@@ -10120,7 +10124,7 @@
       </c>
       <c r="O73" s="31"/>
       <c r="Q73" s="16" t="s">
-        <v>816</v>
+        <v>805</v>
       </c>
       <c r="R73" s="30" t="s">
         <v>75</v>
@@ -10165,7 +10169,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="74" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B74" s="16" t="s">
         <v>798</v>
       </c>
@@ -10189,10 +10193,10 @@
       </c>
       <c r="O74" s="31"/>
       <c r="Q74" s="16" t="s">
-        <v>827</v>
+        <v>816</v>
       </c>
       <c r="R74" s="30" t="s">
-        <v>35</v>
+        <v>75</v>
       </c>
       <c r="S74" s="30" t="s">
         <v>35</v>
@@ -10237,7 +10241,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="75" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B75" s="16" t="s">
         <v>791</v>
       </c>
@@ -10259,10 +10263,10 @@
       </c>
       <c r="O75" s="31"/>
       <c r="Q75" s="16" t="s">
-        <v>1388</v>
+        <v>827</v>
       </c>
       <c r="R75" s="30" t="s">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="S75" s="30" t="s">
         <v>35</v>
@@ -10313,7 +10317,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="76" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B76" s="16" t="s">
         <v>884</v>
       </c>
@@ -10332,7 +10336,7 @@
       <c r="N76" s="31"/>
       <c r="O76" s="31"/>
       <c r="Q76" s="16" t="s">
-        <v>842</v>
+        <v>1388</v>
       </c>
       <c r="R76" s="30" t="s">
         <v>75</v>
@@ -10389,7 +10393,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="77" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B77" s="16" t="s">
         <v>799</v>
       </c>
@@ -10409,7 +10413,7 @@
       <c r="N77" s="31"/>
       <c r="O77" s="31"/>
       <c r="Q77" s="16" t="s">
-        <v>846</v>
+        <v>842</v>
       </c>
       <c r="R77" s="30" t="s">
         <v>75</v>
@@ -10455,7 +10459,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="78" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B78" s="16" t="s">
         <v>889</v>
       </c>
@@ -10475,7 +10479,7 @@
       <c r="N78" s="7"/>
       <c r="O78" s="31"/>
       <c r="Q78" s="16" t="s">
-        <v>852</v>
+        <v>846</v>
       </c>
       <c r="R78" s="30" t="s">
         <v>75</v>
@@ -10532,7 +10536,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="79" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B79" s="16" t="s">
         <v>897</v>
       </c>
@@ -10552,7 +10556,7 @@
       <c r="N79" s="8"/>
       <c r="O79" s="31"/>
       <c r="Q79" s="16" t="s">
-        <v>859</v>
+        <v>852</v>
       </c>
       <c r="R79" s="30" t="s">
         <v>75</v>
@@ -10597,7 +10601,7 @@
         <v>1048</v>
       </c>
     </row>
-    <row r="80" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="J80" s="3"/>
       <c r="K80" s="8" t="s">
         <v>976</v>
@@ -10606,6 +10610,15 @@
         <v>1172</v>
       </c>
       <c r="N80" s="8"/>
+      <c r="Q80" s="16" t="s">
+        <v>859</v>
+      </c>
+      <c r="R80" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="S80" s="30" t="s">
+        <v>35</v>
+      </c>
       <c r="Z80" s="3" t="s">
         <v>987</v>
       </c>
@@ -10637,7 +10650,7 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="81" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B81" s="6" t="s">
         <v>911</v>
       </c>
@@ -10645,15 +10658,6 @@
         <v>1173</v>
       </c>
       <c r="N81" s="7"/>
-      <c r="Q81" s="32" t="s">
-        <v>456</v>
-      </c>
-      <c r="R81" s="6" t="s">
-        <v>405</v>
-      </c>
-      <c r="S81" s="6" t="s">
-        <v>904</v>
-      </c>
       <c r="U81" s="1" t="s">
         <v>1223</v>
       </c>
@@ -10695,7 +10699,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="82" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B82" s="9" t="s">
         <v>918</v>
       </c>
@@ -10706,14 +10710,14 @@
         <v>1174</v>
       </c>
       <c r="N82" s="7"/>
-      <c r="Q82" s="28" t="s">
-        <v>894</v>
-      </c>
-      <c r="R82" s="8" t="s">
-        <v>909</v>
-      </c>
-      <c r="S82" s="8" t="s">
-        <v>910</v>
+      <c r="Q82" s="32" t="s">
+        <v>456</v>
+      </c>
+      <c r="R82" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="S82" s="6" t="s">
+        <v>904</v>
       </c>
       <c r="U82" s="3" t="s">
         <v>1216</v>
@@ -10736,7 +10740,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="83" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B83" s="9" t="s">
         <v>926</v>
       </c>
@@ -10744,13 +10748,13 @@
         <v>927</v>
       </c>
       <c r="Q83" s="28" t="s">
-        <v>903</v>
+        <v>894</v>
       </c>
       <c r="R83" s="8" t="s">
-        <v>916</v>
+        <v>909</v>
       </c>
       <c r="S83" s="8" t="s">
-        <v>917</v>
+        <v>910</v>
       </c>
       <c r="U83" s="3" t="s">
         <v>1217</v>
@@ -10779,7 +10783,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="84" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B84" s="9" t="s">
         <v>934</v>
       </c>
@@ -10796,13 +10800,13 @@
         <v>1308</v>
       </c>
       <c r="Q84" s="28" t="s">
-        <v>908</v>
+        <v>903</v>
       </c>
       <c r="R84" s="8" t="s">
-        <v>924</v>
+        <v>916</v>
       </c>
       <c r="S84" s="8" t="s">
-        <v>925</v>
+        <v>917</v>
       </c>
       <c r="U84" s="3" t="s">
         <v>1221</v>
@@ -10824,7 +10828,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="85" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B85" s="9" t="s">
         <v>939</v>
       </c>
@@ -10841,13 +10845,13 @@
         <v>1310</v>
       </c>
       <c r="Q85" s="28" t="s">
-        <v>915</v>
+        <v>908</v>
       </c>
       <c r="R85" s="8" t="s">
-        <v>932</v>
+        <v>924</v>
       </c>
       <c r="S85" s="8" t="s">
-        <v>933</v>
+        <v>925</v>
       </c>
       <c r="AE85" s="3" t="s">
         <v>1485</v>
@@ -10866,7 +10870,7 @@
         <v>1114</v>
       </c>
     </row>
-    <row r="86" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B86" s="9" t="s">
         <v>943</v>
       </c>
@@ -10882,6 +10886,15 @@
       <c r="O86" s="3" t="s">
         <v>1311</v>
       </c>
+      <c r="Q86" s="28" t="s">
+        <v>915</v>
+      </c>
+      <c r="R86" s="8" t="s">
+        <v>932</v>
+      </c>
+      <c r="S86" s="8" t="s">
+        <v>933</v>
+      </c>
       <c r="AL86" s="8" t="s">
         <v>1433</v>
       </c>
@@ -10895,7 +10908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B87" s="9" t="s">
         <v>946</v>
       </c>
@@ -10911,15 +10924,6 @@
       <c r="O87" s="3" t="s">
         <v>1322</v>
       </c>
-      <c r="Q87" s="6" t="s">
-        <v>1292</v>
-      </c>
-      <c r="R87" s="6" t="s">
-        <v>1293</v>
-      </c>
-      <c r="S87" s="39" t="s">
-        <v>1294</v>
-      </c>
       <c r="AQ87" s="3" t="s">
         <v>1116</v>
       </c>
@@ -10927,7 +10931,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B88" s="9" t="s">
         <v>651</v>
       </c>
@@ -10943,14 +10947,14 @@
       <c r="O88" s="3" t="s">
         <v>1323</v>
       </c>
-      <c r="Q88" s="33">
-        <v>1</v>
-      </c>
-      <c r="R88" s="12" t="s">
-        <v>1295</v>
-      </c>
-      <c r="S88" s="12" t="s">
-        <v>1295</v>
+      <c r="Q88" s="6" t="s">
+        <v>1292</v>
+      </c>
+      <c r="R88" s="6" t="s">
+        <v>1293</v>
+      </c>
+      <c r="S88" s="39" t="s">
+        <v>1294</v>
       </c>
       <c r="AL88" s="6" t="s">
         <v>431</v>
@@ -10962,7 +10966,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B89" s="9" t="s">
         <v>666</v>
       </c>
@@ -10976,13 +10980,13 @@
         <v>1324</v>
       </c>
       <c r="Q89" s="33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R89" s="12" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="S89" s="12" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="AL89" s="8" t="s">
         <v>452</v>
@@ -10994,7 +10998,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="90" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B90" s="9" t="s">
         <v>658</v>
       </c>
@@ -11008,13 +11012,13 @@
         <v>1326</v>
       </c>
       <c r="Q90" s="33">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R90" s="12" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="S90" s="12" t="s">
-        <v>1302</v>
+        <v>1296</v>
       </c>
       <c r="AL90" s="7" t="s">
         <v>464</v>
@@ -11026,7 +11030,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="91" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B91" s="9" t="s">
         <v>951</v>
       </c>
@@ -11040,13 +11044,13 @@
         <v>1325</v>
       </c>
       <c r="Q91" s="33">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R91" s="12" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="S91" s="12" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="AL91" s="8" t="s">
         <v>479</v>
@@ -11058,7 +11062,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="92" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B92" s="9" t="s">
         <v>952</v>
       </c>
@@ -11069,13 +11073,13 @@
         <v>1318</v>
       </c>
       <c r="Q92" s="33">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R92" s="12" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="S92" s="12" t="s">
-        <v>1299</v>
+        <v>1303</v>
       </c>
       <c r="AQ92" s="3" t="s">
         <v>1121</v>
@@ -11084,7 +11088,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="93" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B93" s="9" t="s">
         <v>955</v>
       </c>
@@ -11094,14 +11098,14 @@
       <c r="M93" s="5" t="s">
         <v>1319</v>
       </c>
-      <c r="Q93" s="27">
-        <v>6</v>
+      <c r="Q93" s="33">
+        <v>5</v>
       </c>
       <c r="R93" s="12" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="S93" s="12" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="AL93" s="6" t="s">
         <v>588</v>
@@ -11116,7 +11120,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="94" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B94" s="9" t="s">
         <v>959</v>
       </c>
@@ -11124,13 +11128,13 @@
         <v>960</v>
       </c>
       <c r="Q94" s="27">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="R94" s="12" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="S94" s="12" t="s">
-        <v>1304</v>
+        <v>1300</v>
       </c>
       <c r="AL94" s="7" t="s">
         <v>600</v>
@@ -11148,18 +11152,21 @@
         <v>120</v>
       </c>
     </row>
-    <row r="95" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B95" s="9" t="s">
         <v>962</v>
       </c>
       <c r="C95" s="8" t="s">
         <v>963</v>
       </c>
-      <c r="Q95" s="33">
-        <v>8</v>
+      <c r="Q95" s="27">
+        <v>7</v>
+      </c>
+      <c r="R95" s="12" t="s">
+        <v>1301</v>
       </c>
       <c r="S95" s="12" t="s">
-        <v>1389</v>
+        <v>1304</v>
       </c>
       <c r="AL95" s="7" t="s">
         <v>607</v>
@@ -11177,7 +11184,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="96" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B96" s="9" t="s">
         <v>965</v>
       </c>
@@ -11185,10 +11192,10 @@
         <v>966</v>
       </c>
       <c r="Q96" s="33">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S96" s="12" t="s">
-        <v>1305</v>
+        <v>1389</v>
       </c>
       <c r="AL96" s="25" t="s">
         <v>620</v>
@@ -11206,11 +11213,17 @@
         <v>170</v>
       </c>
     </row>
-    <row r="97" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97"/>
       <c r="B97"/>
       <c r="C97"/>
       <c r="D97"/>
+      <c r="Q97" s="33">
+        <v>9</v>
+      </c>
+      <c r="S97" s="12" t="s">
+        <v>1305</v>
+      </c>
       <c r="AL97" s="7" t="s">
         <v>629</v>
       </c>
@@ -11227,7 +11240,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="98" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98"/>
       <c r="B98"/>
       <c r="C98"/>
@@ -11248,7 +11261,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="99" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99"/>
       <c r="B99"/>
       <c r="C99"/>
@@ -11269,7 +11282,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="100" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100"/>
       <c r="B100"/>
       <c r="C100"/>
@@ -11290,7 +11303,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="101" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101"/>
       <c r="B101"/>
       <c r="C101"/>
@@ -11305,7 +11318,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="102" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102"/>
       <c r="B102"/>
       <c r="C102"/>
@@ -11320,916 +11333,916 @@
         <v>686</v>
       </c>
     </row>
-    <row r="103" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103"/>
       <c r="B103"/>
       <c r="C103"/>
       <c r="D103"/>
     </row>
-    <row r="104" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104"/>
       <c r="B104"/>
       <c r="C104"/>
       <c r="D104"/>
     </row>
-    <row r="105" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105"/>
       <c r="B105"/>
       <c r="C105"/>
       <c r="D105"/>
     </row>
-    <row r="106" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="107" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="108" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="110" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="111" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="112" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="113" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="114" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="115" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="116" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="117" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="118" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="119" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="120" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="121" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="124" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="125" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="126" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="127" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="128" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="129" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="130" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="131" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="132" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="133" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="134" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="135" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="136" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="137" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="138" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="139" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="140" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="141" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="142" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="143" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="144" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="145" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="146" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="147" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="148" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="149" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="150" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="151" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="152" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="153" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="154" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="155" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="156" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="157" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="158" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="159" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="160" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="161" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="162" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="163" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="164" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="165" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="167" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="168" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="169" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="170" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="171" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="172" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="173" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="174" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="175" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="176" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="177" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="178" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="179" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="180" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="181" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="182" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="183" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="184" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="185" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="186" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="187" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="188" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="189" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="190" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="191" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="192" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="193" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="194" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="195" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="196" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="197" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="198" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="199" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="200" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="201" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="202" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="203" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="204" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="205" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="206" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="207" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="208" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="209" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="210" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="211" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="212" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="213" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="214" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="215" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="216" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="217" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="218" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="219" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="220" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="221" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="222" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="223" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="224" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="225" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="226" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="227" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="228" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="229" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="230" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="231" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="232" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="233" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="234" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="235" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="236" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="237" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="238" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="239" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="240" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="241" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="242" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="243" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="244" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="245" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="246" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="247" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="248" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="249" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="250" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="251" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="252" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="253" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="254" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="255" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="256" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="257" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="258" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="259" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="260" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="261" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="262" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="263" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="264" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="265" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="266" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="267" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="268" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="269" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="270" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="271" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="272" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="273" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="274" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="275" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="276" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="277" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="278" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="279" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="280" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="281" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="282" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="283" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="284" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="285" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="286" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="287" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="288" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="289" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="290" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="291" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="292" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="293" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="294" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="295" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="296" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="297" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="298" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="299" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="300" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="301" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="302" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="303" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="304" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="305" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="306" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="307" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="308" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="309" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="310" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="311" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="312" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="313" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="314" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="315" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="316" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="317" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="318" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="319" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="320" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="321" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="322" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="323" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="324" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="325" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="326" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="327" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="328" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="329" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="330" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="331" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="332" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="333" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="334" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="335" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="336" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="337" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="338" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="339" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="340" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="341" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="342" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="343" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="344" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="345" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="346" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="347" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="348" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="349" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="350" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="351" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="352" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="353" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="354" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="355" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="356" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="357" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="358" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="359" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="360" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="361" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="362" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="363" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="364" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="365" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="366" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="367" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="368" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="369" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="370" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="371" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="372" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="373" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="374" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="375" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="376" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="377" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="378" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="379" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="380" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="381" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="382" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="383" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="384" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="385" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="386" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="387" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="388" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="389" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="390" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="391" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="392" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="393" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="394" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="395" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="396" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="397" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="398" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="399" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="400" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="401" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="402" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="403" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="404" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="405" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="406" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="407" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="408" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="409" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="410" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="411" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="412" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="413" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="414" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="415" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="416" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="417" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="418" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="419" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="420" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="421" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="422" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="423" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="424" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="425" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="426" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="427" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="428" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="429" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="430" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="431" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="432" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="433" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="434" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="435" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="436" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="437" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="438" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="439" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="440" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="441" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="442" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="443" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="444" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="445" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="446" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="447" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="448" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="449" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="450" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="451" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="452" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="453" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="454" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="455" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="456" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="457" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="458" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="459" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="460" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="461" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="462" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="463" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="464" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="465" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="466" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="467" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="468" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="469" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="470" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="471" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="472" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="473" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="474" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="475" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="476" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="477" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="478" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="479" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="480" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="481" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="482" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="483" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="484" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="485" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="486" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="487" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="488" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="489" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="490" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="491" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="492" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="493" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="494" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="495" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="496" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="497" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="498" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="499" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="500" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="501" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="502" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="503" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="504" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="505" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="506" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="507" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="508" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="509" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="510" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="511" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="512" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="513" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="514" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="515" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="516" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="517" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="518" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="519" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="520" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="521" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="522" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="523" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="524" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="525" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="526" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="527" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="528" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="529" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="530" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="531" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="532" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="533" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="534" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="535" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="536" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="537" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="538" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="539" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="540" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="541" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="542" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="543" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="544" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="545" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="546" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="547" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="548" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="549" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="550" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="551" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="552" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="553" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="554" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="555" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="556" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="557" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="558" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="559" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="560" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="561" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="562" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="563" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="564" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="565" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="566" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="567" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="568" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="569" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="570" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="571" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="572" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="573" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="574" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="575" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="576" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="577" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="578" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="579" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="580" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="581" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="582" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="583" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="584" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="585" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="586" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="587" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="588" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="589" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="590" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="591" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="592" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="593" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="594" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="595" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="596" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="597" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="598" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="599" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="600" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="601" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="602" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="603" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="604" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="605" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="606" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="607" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="608" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="609" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="610" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="611" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="612" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="613" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="614" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="615" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="616" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="617" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="618" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="619" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="620" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="621" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="622" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="623" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="624" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="625" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="626" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="627" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="628" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="629" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="630" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="631" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="632" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="633" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="634" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="635" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="636" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="637" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="638" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="639" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="640" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="641" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="642" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="643" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="644" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="645" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="646" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="647" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="648" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="649" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="650" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="651" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="652" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="653" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="654" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="655" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="656" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="657" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="658" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="659" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="660" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="661" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="662" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="663" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="664" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="665" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="666" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="667" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="668" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="669" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="670" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="671" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="672" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="673" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="674" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="675" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="676" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="677" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="678" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="679" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="680" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="681" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="682" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="683" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="684" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="685" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="686" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="687" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="688" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="689" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="690" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="691" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="692" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="693" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="694" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="695" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="696" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="697" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="698" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="699" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="700" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="701" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="702" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="703" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="704" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="705" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="706" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="707" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="708" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="709" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="710" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="711" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="712" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="713" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="714" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="715" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="716" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="717" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="718" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="719" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="720" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="721" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="722" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="723" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="724" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="725" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="726" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="727" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="728" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="729" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="730" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="731" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="732" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="733" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="734" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="735" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="736" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="737" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="738" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="739" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="740" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="741" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="742" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="743" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="744" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="745" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="746" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="747" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="748" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="749" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="750" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="751" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="752" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="753" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="754" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="755" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="756" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="757" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="758" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="759" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="760" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="761" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="762" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="763" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="764" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="765" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="766" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="767" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="768" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="769" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="770" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="771" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="772" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="773" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="774" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="775" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="776" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="777" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="778" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="779" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="780" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="781" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="782" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="783" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="784" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="785" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="786" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="787" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="788" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="789" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="790" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="791" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="792" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="793" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="794" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="795" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="796" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="797" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="798" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="799" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="800" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="801" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="802" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="803" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="804" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="805" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="806" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="807" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="808" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="809" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="810" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="811" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="812" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="813" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="814" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="815" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="816" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="817" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="818" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="819" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="820" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="821" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="822" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="823" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="824" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="825" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="826" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="827" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="828" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="829" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="830" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="831" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="832" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="833" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="834" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="835" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="836" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="837" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="838" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="839" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="840" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="841" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="842" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="843" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="844" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="845" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="846" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="847" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="848" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="849" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="850" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="851" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="852" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="853" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="854" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="855" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="856" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="857" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="858" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="859" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="860" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="861" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="862" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="863" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="864" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="865" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="866" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="867" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="868" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="869" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="870" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="871" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="872" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="873" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="874" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="875" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="876" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="877" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="878" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="879" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="880" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="881" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="882" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="883" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="884" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="885" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="886" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="887" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="888" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="889" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="890" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="891" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="892" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="893" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="894" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="895" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="896" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="897" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="898" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="899" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="900" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="901" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="902" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="903" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="904" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="905" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="906" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="907" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="908" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="909" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="910" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="911" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="912" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="913" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="914" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="915" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="916" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="917" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="918" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="919" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="920" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="921" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="922" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="923" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="924" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="925" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="926" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="927" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="928" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="929" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="930" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="931" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="932" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="933" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="934" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="935" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="936" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="937" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="938" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="939" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="940" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="941" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="942" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="943" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="944" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="945" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="946" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="947" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="948" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="949" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="950" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="951" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="952" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="953" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="954" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="955" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="956" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="957" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="958" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="959" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="960" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="961" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="962" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="963" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="964" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="965" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="966" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="967" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="968" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="969" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="970" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="971" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="972" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="973" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="974" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="975" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="976" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="977" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="978" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="979" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="980" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="981" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="982" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="983" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="984" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="107" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="108" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="109" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="110" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="111" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="112" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="113" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="114" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="115" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="117" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="118" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="119" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="120" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="121" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="122" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="123" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="124" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="125" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="126" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="127" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="128" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="129" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="130" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="131" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="132" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="133" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="134" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="135" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="136" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="137" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="138" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="139" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="140" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="141" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="142" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="143" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="144" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="145" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="146" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="147" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="148" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="149" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="150" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="151" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="152" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="153" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="154" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="155" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="156" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="157" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="158" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="159" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="160" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="161" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="162" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="163" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="164" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="165" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="167" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="168" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="169" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="170" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="171" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="172" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="173" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="174" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="175" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="176" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="177" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="178" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="179" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="180" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="181" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="182" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="183" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="184" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="185" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="186" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="187" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="188" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="189" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="190" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="191" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="192" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="193" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="194" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="195" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="196" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="197" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="198" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="199" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="200" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="201" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="202" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="203" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="204" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="205" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="206" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="207" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="208" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="209" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="210" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="211" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="212" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="213" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="214" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="215" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="216" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="217" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="218" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="219" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="220" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="221" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="222" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="223" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="224" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="225" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="226" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="227" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="228" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="229" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="230" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="231" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="232" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="233" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="234" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="235" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="236" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="237" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="238" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="239" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="240" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="241" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="242" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="243" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="244" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="245" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="246" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="247" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="248" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="249" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="250" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="251" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="252" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="253" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="254" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="255" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="256" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="257" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="258" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="259" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="260" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="261" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="262" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="263" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="264" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="265" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="266" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="267" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="268" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="269" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="270" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="271" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="272" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="273" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="274" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="275" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="276" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="277" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="278" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="279" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="280" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="281" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="282" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="283" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="284" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="285" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="286" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="287" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="288" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="289" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="290" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="291" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="292" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="293" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="294" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="295" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="296" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="297" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="298" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="299" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="300" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="301" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="302" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="303" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="304" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="305" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="306" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="307" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="308" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="309" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="310" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="311" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="312" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="313" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="314" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="315" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="316" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="317" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="318" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="319" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="320" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="321" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="322" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="323" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="324" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="325" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="326" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="327" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="328" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="329" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="330" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="331" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="332" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="333" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="334" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="335" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="336" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="337" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="338" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="339" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="340" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="341" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="342" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="343" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="344" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="345" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="346" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="347" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="348" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="349" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="350" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="351" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="352" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="353" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="354" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="355" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="356" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="357" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="358" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="359" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="360" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="361" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="362" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="363" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="364" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="365" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="366" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="367" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="368" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="369" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="370" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="371" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="372" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="373" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="374" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="375" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="376" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="377" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="378" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="379" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="380" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="381" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="382" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="383" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="384" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="385" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="386" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="387" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="388" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="389" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="390" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="391" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="392" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="393" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="394" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="395" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="396" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="397" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="398" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="399" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="400" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="401" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="402" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="403" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="404" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="405" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="406" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="407" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="408" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="409" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="410" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="411" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="412" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="413" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="414" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="415" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="416" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="417" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="418" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="419" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="420" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="421" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="422" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="423" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="424" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="425" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="426" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="427" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="428" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="429" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="430" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="431" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="432" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="433" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="434" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="435" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="436" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="437" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="438" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="439" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="440" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="441" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="442" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="443" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="444" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="445" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="446" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="447" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="448" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="449" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="450" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="451" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="452" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="453" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="454" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="455" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="456" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="457" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="458" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="459" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="460" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="461" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="462" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="463" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="464" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="465" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="466" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="467" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="468" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="469" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="470" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="471" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="472" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="473" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="474" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="475" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="476" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="477" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="478" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="479" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="480" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="481" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="482" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="483" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="484" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="485" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="486" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="487" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="488" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="489" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="490" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="491" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="492" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="493" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="494" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="495" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="496" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="497" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="498" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="499" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="500" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="501" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="502" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="503" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="504" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="505" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="506" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="507" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="508" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="509" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="510" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="511" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="512" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="513" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="514" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="515" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="516" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="517" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="518" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="519" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="520" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="521" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="522" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="523" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="524" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="525" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="526" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="527" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="528" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="529" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="530" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="531" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="532" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="533" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="534" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="535" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="536" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="537" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="538" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="539" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="540" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="541" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="542" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="543" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="544" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="545" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="546" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="547" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="548" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="549" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="550" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="551" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="552" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="553" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="554" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="555" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="556" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="557" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="558" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="559" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="560" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="561" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="562" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="563" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="564" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="565" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="566" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="567" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="568" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="569" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="570" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="571" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="572" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="573" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="574" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="575" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="576" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="577" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="578" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="579" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="580" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="581" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="582" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="583" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="584" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="585" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="586" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="587" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="588" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="589" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="590" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="591" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="592" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="593" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="594" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="595" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="596" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="597" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="598" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="599" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="600" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="601" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="602" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="603" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="604" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="605" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="606" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="607" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="608" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="609" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="610" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="611" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="612" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="613" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="614" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="615" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="616" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="617" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="618" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="619" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="620" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="621" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="622" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="623" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="624" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="625" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="626" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="627" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="628" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="629" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="630" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="631" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="632" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="633" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="634" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="635" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="636" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="637" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="638" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="639" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="640" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="641" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="642" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="643" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="644" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="645" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="646" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="647" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="648" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="649" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="650" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="651" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="652" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="653" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="654" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="655" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="656" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="657" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="658" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="659" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="660" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="661" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="662" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="663" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="664" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="665" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="666" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="667" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="668" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="669" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="670" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="671" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="672" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="673" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="674" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="675" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="676" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="677" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="678" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="679" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="680" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="681" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="682" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="683" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="684" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="685" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="686" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="687" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="688" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="689" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="690" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="691" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="692" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="693" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="694" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="695" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="696" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="697" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="698" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="699" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="700" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="701" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="702" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="703" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="704" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="705" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="706" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="707" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="708" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="709" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="710" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="711" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="712" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="713" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="714" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="715" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="716" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="717" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="718" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="719" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="720" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="721" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="722" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="723" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="724" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="725" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="726" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="727" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="728" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="729" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="730" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="731" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="732" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="733" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="734" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="735" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="736" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="737" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="738" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="739" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="740" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="741" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="742" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="743" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="744" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="745" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="746" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="747" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="748" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="749" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="750" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="751" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="752" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="753" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="754" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="755" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="756" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="757" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="758" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="759" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="760" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="761" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="762" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="763" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="764" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="765" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="766" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="767" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="768" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="769" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="770" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="771" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="772" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="773" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="774" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="775" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="776" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="777" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="778" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="779" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="780" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="781" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="782" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="783" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="784" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="785" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="786" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="787" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="788" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="789" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="790" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="791" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="792" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="793" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="794" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="795" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="796" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="797" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="798" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="799" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="800" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="801" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="802" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="803" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="804" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="805" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="806" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="807" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="808" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="809" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="810" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="811" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="812" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="813" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="814" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="815" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="816" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="817" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="818" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="819" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="820" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="821" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="822" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="823" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="824" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="825" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="826" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="827" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="828" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="829" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="830" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="831" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="832" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="833" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="834" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="835" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="836" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="837" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="838" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="839" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="840" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="841" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="842" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="843" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="844" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="845" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="846" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="847" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="848" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="849" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="850" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="851" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="852" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="853" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="854" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="855" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="856" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="857" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="858" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="859" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="860" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="861" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="862" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="863" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="864" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="865" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="866" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="867" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="868" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="869" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="870" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="871" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="872" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="873" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="874" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="875" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="876" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="877" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="878" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="879" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="880" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="881" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="882" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="883" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="884" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="885" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="886" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="887" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="888" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="889" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="890" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="891" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="892" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="893" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="894" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="895" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="896" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="897" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="898" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="899" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="900" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="901" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="902" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="903" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="904" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="905" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="906" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="907" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="908" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="909" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="910" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="911" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="912" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="913" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="914" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="915" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="916" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="917" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="918" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="919" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="920" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="921" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="922" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="923" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="924" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="925" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="926" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="927" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="928" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="929" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="930" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="931" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="932" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="933" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="934" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="935" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="936" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="937" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="938" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="939" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="940" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="941" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="942" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="943" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="944" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="945" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="946" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="947" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="948" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="949" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="950" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="951" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="952" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="953" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="954" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="955" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="956" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="957" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="958" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="959" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="960" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="961" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="962" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="963" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="964" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="965" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="966" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="967" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="968" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="969" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="970" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="971" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="972" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="973" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="974" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="975" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="976" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="977" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="978" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="979" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="980" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="981" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="982" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="983" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="984" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>